<commit_message>
implementacion completa de reporte tarjeta kardex para productos
</commit_message>
<xml_diff>
--- a/Files/Reporte_Stock/900987412_3/Reporte_Stock_MAS LOGISTICA_1.xlsx
+++ b/Files/Reporte_Stock/900987412_3/Reporte_Stock_MAS LOGISTICA_1.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="634">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="633">
   <si>
     <t>REPORTE STOCK CLIENTE MAS LOGISTICA
 SUC. IMPORTACIONES LANCH</t>
@@ -66,7 +66,7 @@
     <t>Estuche Spigen Liquid Air Apple iPhone iPhone SE 2020 / 8 / 7 - Negro</t>
   </si>
   <si>
-    <t>2A</t>
+    <t>1F</t>
   </si>
   <si>
     <t>565CS20828</t>
@@ -147,7 +147,7 @@
     <t>3C</t>
   </si>
   <si>
-    <t>NA</t>
+    <t>SERT0002</t>
   </si>
   <si>
     <t>Estuche VRS Crystal Chrome Huawei Honor 8X Max - Claro</t>
@@ -310,9 +310,6 @@
   </si>
   <si>
     <t>Vidrio Flexible Ringke DualEasyFull Apple Iphone 11 Pro Max - (1+1)</t>
-  </si>
-  <si>
-    <t>1F</t>
   </si>
   <si>
     <t>ESSG0001</t>
@@ -2011,7 +2008,7 @@
       <xdr:row>0</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
-    <xdr:ext cx="1238250" cy="571500"/>
+    <xdr:ext cx="2057400" cy="952500"/>
     <xdr:pic>
       <xdr:nvPicPr>
         <xdr:cNvPr id="1" name="Logo" descr="Logo"/>
@@ -2342,7 +2339,7 @@
     <col min="5" max="5" width="9" customWidth="true" style="0"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" customHeight="1" ht="60">
+    <row r="1" spans="1:5" customHeight="1" ht="70">
       <c r="A1" s="1"/>
       <c r="B1" s="1"/>
       <c r="C1" s="2" t="s">
@@ -2399,7 +2396,7 @@
         <v>11</v>
       </c>
       <c r="E4">
-        <v>13</v>
+        <v>16</v>
       </c>
     </row>
     <row r="5" spans="1:5">
@@ -2416,7 +2413,7 @@
         <v>11</v>
       </c>
       <c r="E5">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="6" spans="1:5">
@@ -2433,7 +2430,7 @@
         <v>16</v>
       </c>
       <c r="E6">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="7" spans="1:5">
@@ -2484,7 +2481,7 @@
         <v>24</v>
       </c>
       <c r="E9">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="10" spans="1:5">
@@ -2535,7 +2532,7 @@
         <v>32</v>
       </c>
       <c r="E12">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="13" spans="1:5">
@@ -2552,7 +2549,7 @@
         <v>35</v>
       </c>
       <c r="E13">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="14" spans="1:5">
@@ -2569,7 +2566,7 @@
         <v>24</v>
       </c>
       <c r="E14">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="15" spans="1:5">
@@ -2603,7 +2600,7 @@
         <v>42</v>
       </c>
       <c r="E16">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" spans="1:5">
@@ -2637,7 +2634,7 @@
         <v>48</v>
       </c>
       <c r="E18">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="19" spans="1:5">
@@ -2688,7 +2685,7 @@
         <v>56</v>
       </c>
       <c r="E21">
-        <v>39</v>
+        <v>40</v>
       </c>
     </row>
     <row r="22" spans="1:5">
@@ -2705,7 +2702,7 @@
         <v>11</v>
       </c>
       <c r="E22">
-        <v>7</v>
+        <v>10</v>
       </c>
     </row>
     <row r="23" spans="1:5">
@@ -2756,7 +2753,7 @@
         <v>65</v>
       </c>
       <c r="E25">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="26" spans="1:5">
@@ -2773,7 +2770,7 @@
         <v>68</v>
       </c>
       <c r="E26">
-        <v>27</v>
+        <v>30</v>
       </c>
     </row>
     <row r="27" spans="1:5">
@@ -2841,7 +2838,7 @@
         <v>79</v>
       </c>
       <c r="E30">
-        <v>20</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5">
@@ -2858,7 +2855,7 @@
         <v>82</v>
       </c>
       <c r="E31">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="32" spans="1:5">
@@ -2875,7 +2872,7 @@
         <v>19</v>
       </c>
       <c r="E32">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="33" spans="1:5">
@@ -2892,7 +2889,7 @@
         <v>87</v>
       </c>
       <c r="E33">
-        <v>48</v>
+        <v>50</v>
       </c>
     </row>
     <row r="34" spans="1:5">
@@ -2957,7 +2954,7 @@
         <v>97</v>
       </c>
       <c r="D37" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E37">
         <v>20</v>
@@ -2968,13 +2965,13 @@
         <v>8809628564169</v>
       </c>
       <c r="B38" t="s">
+        <v>98</v>
+      </c>
+      <c r="C38" t="s">
         <v>99</v>
       </c>
-      <c r="C38" t="s">
+      <c r="D38" t="s">
         <v>100</v>
-      </c>
-      <c r="D38" t="s">
-        <v>101</v>
       </c>
       <c r="E38">
         <v>15</v>
@@ -2985,16 +2982,16 @@
         <v>8809628565333</v>
       </c>
       <c r="B39" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="C39" t="s">
         <v>58</v>
       </c>
       <c r="D39" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E39">
-        <v>37</v>
+        <v>40</v>
       </c>
     </row>
     <row r="40" spans="1:5">
@@ -3002,16 +2999,16 @@
         <v>8809628566316</v>
       </c>
       <c r="B40" t="s">
+        <v>102</v>
+      </c>
+      <c r="C40" t="s">
         <v>103</v>
       </c>
-      <c r="C40" t="s">
-        <v>104</v>
-      </c>
       <c r="D40" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E40">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="41" spans="1:5">
@@ -3019,16 +3016,16 @@
         <v>8809628566590</v>
       </c>
       <c r="B41" t="s">
+        <v>104</v>
+      </c>
+      <c r="C41" t="s">
         <v>105</v>
-      </c>
-      <c r="C41" t="s">
-        <v>106</v>
       </c>
       <c r="D41" t="s">
         <v>90</v>
       </c>
       <c r="E41">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="42" spans="1:5">
@@ -3036,10 +3033,10 @@
         <v>8809628566927</v>
       </c>
       <c r="B42" t="s">
+        <v>106</v>
+      </c>
+      <c r="C42" t="s">
         <v>107</v>
-      </c>
-      <c r="C42" t="s">
-        <v>108</v>
       </c>
       <c r="D42" t="s">
         <v>82</v>
@@ -3053,16 +3050,16 @@
         <v>8809628567122</v>
       </c>
       <c r="B43" t="s">
+        <v>108</v>
+      </c>
+      <c r="C43" t="s">
         <v>109</v>
-      </c>
-      <c r="C43" t="s">
-        <v>110</v>
       </c>
       <c r="D43" t="s">
         <v>71</v>
       </c>
       <c r="E43">
-        <v>13</v>
+        <v>20</v>
       </c>
     </row>
     <row r="44" spans="1:5">
@@ -3070,16 +3067,16 @@
         <v>8809628567207</v>
       </c>
       <c r="B44" t="s">
+        <v>110</v>
+      </c>
+      <c r="C44" t="s">
         <v>111</v>
       </c>
-      <c r="C44" t="s">
+      <c r="D44" t="s">
         <v>112</v>
       </c>
-      <c r="D44" t="s">
-        <v>113</v>
-      </c>
       <c r="E44">
-        <v>19</v>
+        <v>25</v>
       </c>
     </row>
     <row r="45" spans="1:5">
@@ -3087,16 +3084,16 @@
         <v>8809628567276</v>
       </c>
       <c r="B45" t="s">
+        <v>113</v>
+      </c>
+      <c r="C45" t="s">
         <v>114</v>
       </c>
-      <c r="C45" t="s">
+      <c r="D45" t="s">
         <v>115</v>
       </c>
-      <c r="D45" t="s">
-        <v>116</v>
-      </c>
       <c r="E45">
-        <v>4</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:5">
@@ -3104,16 +3101,16 @@
         <v>8809628567290</v>
       </c>
       <c r="B46" t="s">
+        <v>116</v>
+      </c>
+      <c r="C46" t="s">
         <v>117</v>
       </c>
-      <c r="C46" t="s">
+      <c r="D46" t="s">
         <v>118</v>
       </c>
-      <c r="D46" t="s">
-        <v>119</v>
-      </c>
       <c r="E46">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="47" spans="1:5">
@@ -3121,10 +3118,10 @@
         <v>8809628567375</v>
       </c>
       <c r="B47" t="s">
+        <v>119</v>
+      </c>
+      <c r="C47" t="s">
         <v>120</v>
-      </c>
-      <c r="C47" t="s">
-        <v>121</v>
       </c>
       <c r="D47" t="s">
         <v>40</v>
@@ -3138,13 +3135,13 @@
         <v>8809628567450</v>
       </c>
       <c r="B48" t="s">
+        <v>121</v>
+      </c>
+      <c r="C48" t="s">
         <v>122</v>
       </c>
-      <c r="C48" t="s">
+      <c r="D48" t="s">
         <v>123</v>
-      </c>
-      <c r="D48" t="s">
-        <v>124</v>
       </c>
       <c r="E48">
         <v>20</v>
@@ -3155,13 +3152,13 @@
         <v>8809628567474</v>
       </c>
       <c r="B49" t="s">
+        <v>124</v>
+      </c>
+      <c r="C49" t="s">
         <v>125</v>
       </c>
-      <c r="C49" t="s">
+      <c r="D49" t="s">
         <v>126</v>
-      </c>
-      <c r="D49" t="s">
-        <v>127</v>
       </c>
       <c r="E49">
         <v>25</v>
@@ -3172,13 +3169,13 @@
         <v>8809628567498</v>
       </c>
       <c r="B50" t="s">
+        <v>127</v>
+      </c>
+      <c r="C50" t="s">
         <v>128</v>
       </c>
-      <c r="C50" t="s">
-        <v>129</v>
-      </c>
       <c r="D50" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E50">
         <v>22</v>
@@ -3189,10 +3186,10 @@
         <v>8809628568648</v>
       </c>
       <c r="B51" t="s">
+        <v>129</v>
+      </c>
+      <c r="C51" t="s">
         <v>130</v>
-      </c>
-      <c r="C51" t="s">
-        <v>131</v>
       </c>
       <c r="D51" t="s">
         <v>87</v>
@@ -3206,16 +3203,16 @@
         <v>8809628568730</v>
       </c>
       <c r="B52" t="s">
+        <v>131</v>
+      </c>
+      <c r="C52" t="s">
         <v>132</v>
       </c>
-      <c r="C52" t="s">
+      <c r="D52" t="s">
         <v>133</v>
       </c>
-      <c r="D52" t="s">
-        <v>134</v>
-      </c>
       <c r="E52">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="53" spans="1:5">
@@ -3223,16 +3220,16 @@
         <v>8809628568853</v>
       </c>
       <c r="B53" t="s">
+        <v>134</v>
+      </c>
+      <c r="C53" t="s">
         <v>135</v>
-      </c>
-      <c r="C53" t="s">
-        <v>136</v>
       </c>
       <c r="D53" t="s">
         <v>82</v>
       </c>
       <c r="E53">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="54" spans="1:5">
@@ -3240,16 +3237,16 @@
         <v>8809628568877</v>
       </c>
       <c r="B54" t="s">
+        <v>136</v>
+      </c>
+      <c r="C54" t="s">
         <v>137</v>
       </c>
-      <c r="C54" t="s">
+      <c r="D54" t="s">
         <v>138</v>
       </c>
-      <c r="D54" t="s">
-        <v>139</v>
-      </c>
       <c r="E54">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="55" spans="1:5">
@@ -3257,13 +3254,13 @@
         <v>8809628568969</v>
       </c>
       <c r="B55" t="s">
+        <v>139</v>
+      </c>
+      <c r="C55" t="s">
         <v>140</v>
       </c>
-      <c r="C55" t="s">
-        <v>141</v>
-      </c>
       <c r="D55" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E55">
         <v>44</v>
@@ -3274,13 +3271,13 @@
         <v>8809628569089</v>
       </c>
       <c r="B56" t="s">
+        <v>141</v>
+      </c>
+      <c r="C56" t="s">
         <v>142</v>
       </c>
-      <c r="C56" t="s">
+      <c r="D56" t="s">
         <v>143</v>
-      </c>
-      <c r="D56" t="s">
-        <v>144</v>
       </c>
       <c r="E56">
         <v>22</v>
@@ -3291,13 +3288,13 @@
         <v>8809628569102</v>
       </c>
       <c r="B57" t="s">
+        <v>144</v>
+      </c>
+      <c r="C57" t="s">
         <v>145</v>
       </c>
-      <c r="C57" t="s">
-        <v>146</v>
-      </c>
       <c r="D57" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E57">
         <v>25</v>
@@ -3308,13 +3305,13 @@
         <v>8809628569195</v>
       </c>
       <c r="B58" t="s">
+        <v>146</v>
+      </c>
+      <c r="C58" t="s">
         <v>147</v>
       </c>
-      <c r="C58" t="s">
-        <v>148</v>
-      </c>
       <c r="D58" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E58">
         <v>20</v>
@@ -3325,16 +3322,16 @@
         <v>8809628569928</v>
       </c>
       <c r="B59" t="s">
+        <v>148</v>
+      </c>
+      <c r="C59" t="s">
         <v>149</v>
-      </c>
-      <c r="C59" t="s">
-        <v>150</v>
       </c>
       <c r="D59" t="s">
         <v>11</v>
       </c>
       <c r="E59">
-        <v>29</v>
+        <v>30</v>
       </c>
     </row>
     <row r="60" spans="1:5">
@@ -3342,10 +3339,10 @@
         <v>8809628569959</v>
       </c>
       <c r="B60" t="s">
+        <v>150</v>
+      </c>
+      <c r="C60" t="s">
         <v>151</v>
-      </c>
-      <c r="C60" t="s">
-        <v>152</v>
       </c>
       <c r="D60" t="s">
         <v>32</v>
@@ -3359,10 +3356,10 @@
         <v>8809640250392</v>
       </c>
       <c r="B61" t="s">
+        <v>152</v>
+      </c>
+      <c r="C61" t="s">
         <v>153</v>
-      </c>
-      <c r="C61" t="s">
-        <v>154</v>
       </c>
       <c r="D61" t="s">
         <v>35</v>
@@ -3376,13 +3373,13 @@
         <v>8809640251320</v>
       </c>
       <c r="B62" t="s">
+        <v>154</v>
+      </c>
+      <c r="C62" t="s">
         <v>155</v>
       </c>
-      <c r="C62" t="s">
+      <c r="D62" t="s">
         <v>156</v>
-      </c>
-      <c r="D62" t="s">
-        <v>157</v>
       </c>
       <c r="E62">
         <v>30</v>
@@ -3393,10 +3390,10 @@
         <v>8809640252266</v>
       </c>
       <c r="B63" t="s">
+        <v>157</v>
+      </c>
+      <c r="C63" t="s">
         <v>158</v>
-      </c>
-      <c r="C63" t="s">
-        <v>159</v>
       </c>
       <c r="D63" t="s">
         <v>19</v>
@@ -3410,13 +3407,13 @@
         <v>8809640258718</v>
       </c>
       <c r="B64" t="s">
+        <v>159</v>
+      </c>
+      <c r="C64" t="s">
         <v>160</v>
       </c>
-      <c r="C64" t="s">
-        <v>161</v>
-      </c>
       <c r="D64" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E64">
         <v>19</v>
@@ -3427,13 +3424,13 @@
         <v>8809640259739</v>
       </c>
       <c r="B65" t="s">
+        <v>161</v>
+      </c>
+      <c r="C65" t="s">
         <v>162</v>
       </c>
-      <c r="C65" t="s">
-        <v>163</v>
-      </c>
       <c r="D65" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E65">
         <v>10</v>
@@ -3444,16 +3441,16 @@
         <v>8809640259784</v>
       </c>
       <c r="B66" t="s">
+        <v>163</v>
+      </c>
+      <c r="C66" t="s">
         <v>164</v>
       </c>
-      <c r="C66" t="s">
+      <c r="D66" t="s">
         <v>165</v>
       </c>
-      <c r="D66" t="s">
-        <v>166</v>
-      </c>
       <c r="E66">
-        <v>9</v>
+        <v>15</v>
       </c>
     </row>
     <row r="67" spans="1:5">
@@ -3461,16 +3458,16 @@
         <v>8809659042018</v>
       </c>
       <c r="B67" t="s">
+        <v>166</v>
+      </c>
+      <c r="C67" t="s">
         <v>167</v>
-      </c>
-      <c r="C67" t="s">
-        <v>168</v>
       </c>
       <c r="D67" t="s">
         <v>24</v>
       </c>
       <c r="E67">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="68" spans="1:5">
@@ -3478,16 +3475,16 @@
         <v>8809659042049</v>
       </c>
       <c r="B68" t="s">
+        <v>168</v>
+      </c>
+      <c r="C68" t="s">
         <v>169</v>
       </c>
-      <c r="C68" t="s">
+      <c r="D68" t="s">
         <v>170</v>
       </c>
-      <c r="D68" t="s">
-        <v>171</v>
-      </c>
       <c r="E68">
-        <v>15</v>
+        <v>17</v>
       </c>
     </row>
     <row r="69" spans="1:5">
@@ -3495,16 +3492,16 @@
         <v>8809659042070</v>
       </c>
       <c r="B69" t="s">
+        <v>171</v>
+      </c>
+      <c r="C69" t="s">
         <v>172</v>
-      </c>
-      <c r="C69" t="s">
-        <v>173</v>
       </c>
       <c r="D69" t="s">
         <v>71</v>
       </c>
       <c r="E69">
-        <v>6</v>
+        <v>25</v>
       </c>
     </row>
     <row r="70" spans="1:5">
@@ -3512,10 +3509,10 @@
         <v>8809659042131</v>
       </c>
       <c r="B70" t="s">
+        <v>173</v>
+      </c>
+      <c r="C70" t="s">
         <v>174</v>
-      </c>
-      <c r="C70" t="s">
-        <v>175</v>
       </c>
       <c r="D70" t="s">
         <v>95</v>
@@ -3529,16 +3526,16 @@
         <v>8809659042162</v>
       </c>
       <c r="B71" t="s">
+        <v>175</v>
+      </c>
+      <c r="C71" t="s">
         <v>176</v>
-      </c>
-      <c r="C71" t="s">
-        <v>177</v>
       </c>
       <c r="D71" t="s">
         <v>24</v>
       </c>
       <c r="E71">
-        <v>45</v>
+        <v>50</v>
       </c>
     </row>
     <row r="72" spans="1:5">
@@ -3546,16 +3543,16 @@
         <v>8809659042636</v>
       </c>
       <c r="B72" t="s">
+        <v>177</v>
+      </c>
+      <c r="C72" t="s">
         <v>178</v>
-      </c>
-      <c r="C72" t="s">
-        <v>179</v>
       </c>
       <c r="D72" t="s">
         <v>42</v>
       </c>
       <c r="E72">
-        <v>14</v>
+        <v>18</v>
       </c>
     </row>
     <row r="73" spans="1:5">
@@ -3563,10 +3560,10 @@
         <v>8809659042728</v>
       </c>
       <c r="B73" t="s">
+        <v>179</v>
+      </c>
+      <c r="C73" t="s">
         <v>180</v>
-      </c>
-      <c r="C73" t="s">
-        <v>181</v>
       </c>
       <c r="D73" t="s">
         <v>87</v>
@@ -3580,16 +3577,16 @@
         <v>8809659043152</v>
       </c>
       <c r="B74" t="s">
+        <v>181</v>
+      </c>
+      <c r="C74" t="s">
         <v>182</v>
-      </c>
-      <c r="C74" t="s">
-        <v>183</v>
       </c>
       <c r="D74" t="s">
         <v>35</v>
       </c>
       <c r="E74">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="75" spans="1:5">
@@ -3597,16 +3594,16 @@
         <v>8809659044012</v>
       </c>
       <c r="B75" t="s">
+        <v>183</v>
+      </c>
+      <c r="C75" t="s">
         <v>184</v>
       </c>
-      <c r="C75" t="s">
-        <v>185</v>
-      </c>
       <c r="D75" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E75">
-        <v>9</v>
+        <v>50</v>
       </c>
     </row>
     <row r="76" spans="1:5">
@@ -3614,16 +3611,16 @@
         <v>8809659044043</v>
       </c>
       <c r="B76" t="s">
+        <v>185</v>
+      </c>
+      <c r="C76" t="s">
         <v>186</v>
       </c>
-      <c r="C76" t="s">
-        <v>187</v>
-      </c>
       <c r="D76" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E76">
-        <v>3</v>
+        <v>40</v>
       </c>
     </row>
     <row r="77" spans="1:5">
@@ -3631,13 +3628,13 @@
         <v>8809659044098</v>
       </c>
       <c r="B77" t="s">
+        <v>187</v>
+      </c>
+      <c r="C77" t="s">
         <v>188</v>
       </c>
-      <c r="C77" t="s">
-        <v>189</v>
-      </c>
       <c r="D77" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E77">
         <v>17</v>
@@ -3648,13 +3645,13 @@
         <v>8809659044128</v>
       </c>
       <c r="B78" t="s">
+        <v>189</v>
+      </c>
+      <c r="C78" t="s">
         <v>190</v>
       </c>
-      <c r="C78" t="s">
+      <c r="D78" t="s">
         <v>191</v>
-      </c>
-      <c r="D78" t="s">
-        <v>192</v>
       </c>
       <c r="E78">
         <v>25</v>
@@ -3665,13 +3662,13 @@
         <v>8809659044159</v>
       </c>
       <c r="B79" t="s">
+        <v>192</v>
+      </c>
+      <c r="C79" t="s">
         <v>193</v>
       </c>
-      <c r="C79" t="s">
-        <v>194</v>
-      </c>
       <c r="D79" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E79">
         <v>17</v>
@@ -3682,16 +3679,16 @@
         <v>8809659044258</v>
       </c>
       <c r="B80" t="s">
+        <v>194</v>
+      </c>
+      <c r="C80" t="s">
         <v>195</v>
       </c>
-      <c r="C80" t="s">
-        <v>196</v>
-      </c>
       <c r="D80" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E80">
-        <v>3</v>
+        <v>15</v>
       </c>
     </row>
     <row r="81" spans="1:5">
@@ -3699,16 +3696,16 @@
         <v>8809659044418</v>
       </c>
       <c r="B81" t="s">
+        <v>196</v>
+      </c>
+      <c r="C81" t="s">
         <v>197</v>
       </c>
-      <c r="C81" t="s">
-        <v>198</v>
-      </c>
       <c r="D81" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E81">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="82" spans="1:5">
@@ -3716,13 +3713,13 @@
         <v>8809659045507</v>
       </c>
       <c r="B82" t="s">
+        <v>198</v>
+      </c>
+      <c r="C82" t="s">
         <v>199</v>
       </c>
-      <c r="C82" t="s">
-        <v>200</v>
-      </c>
       <c r="D82" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E82">
         <v>13</v>
@@ -3733,13 +3730,13 @@
         <v>8809659045538</v>
       </c>
       <c r="B83" t="s">
+        <v>200</v>
+      </c>
+      <c r="C83" t="s">
         <v>201</v>
       </c>
-      <c r="C83" t="s">
+      <c r="D83" t="s">
         <v>202</v>
-      </c>
-      <c r="D83" t="s">
-        <v>203</v>
       </c>
       <c r="E83">
         <v>29</v>
@@ -3750,16 +3747,16 @@
         <v>8809659045668</v>
       </c>
       <c r="B84" t="s">
+        <v>203</v>
+      </c>
+      <c r="C84" t="s">
         <v>204</v>
-      </c>
-      <c r="C84" t="s">
-        <v>205</v>
       </c>
       <c r="D84" t="s">
         <v>29</v>
       </c>
       <c r="E84">
-        <v>8</v>
+        <v>25</v>
       </c>
     </row>
     <row r="85" spans="1:5">
@@ -3767,16 +3764,16 @@
         <v>8809659045828</v>
       </c>
       <c r="B85" t="s">
+        <v>205</v>
+      </c>
+      <c r="C85" t="s">
         <v>206</v>
       </c>
-      <c r="C85" t="s">
-        <v>207</v>
-      </c>
       <c r="D85" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E85">
-        <v>23</v>
+        <v>25</v>
       </c>
     </row>
     <row r="86" spans="1:5">
@@ -3784,16 +3781,16 @@
         <v>8809659045859</v>
       </c>
       <c r="B86" t="s">
+        <v>207</v>
+      </c>
+      <c r="C86" t="s">
         <v>208</v>
       </c>
-      <c r="C86" t="s">
+      <c r="D86" t="s">
         <v>209</v>
       </c>
-      <c r="D86" t="s">
-        <v>210</v>
-      </c>
       <c r="E86">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="87" spans="1:5">
@@ -3801,16 +3798,16 @@
         <v>8809659045880</v>
       </c>
       <c r="B87" t="s">
+        <v>210</v>
+      </c>
+      <c r="C87" t="s">
         <v>211</v>
-      </c>
-      <c r="C87" t="s">
-        <v>212</v>
       </c>
       <c r="D87" t="s">
         <v>56</v>
       </c>
       <c r="E87">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="88" spans="1:5">
@@ -3818,13 +3815,13 @@
         <v>8809659046139</v>
       </c>
       <c r="B88" t="s">
+        <v>212</v>
+      </c>
+      <c r="C88" t="s">
         <v>213</v>
       </c>
-      <c r="C88" t="s">
+      <c r="D88" t="s">
         <v>214</v>
-      </c>
-      <c r="D88" t="s">
-        <v>215</v>
       </c>
       <c r="E88">
         <v>30</v>
@@ -3835,16 +3832,16 @@
         <v>8809659047228</v>
       </c>
       <c r="B89" t="s">
+        <v>215</v>
+      </c>
+      <c r="C89" t="s">
         <v>216</v>
       </c>
-      <c r="C89" t="s">
-        <v>217</v>
-      </c>
       <c r="D89" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E89">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="90" spans="1:5">
@@ -3852,13 +3849,13 @@
         <v>8809659047488</v>
       </c>
       <c r="B90" t="s">
+        <v>217</v>
+      </c>
+      <c r="C90" t="s">
         <v>218</v>
       </c>
-      <c r="C90" t="s">
+      <c r="D90" t="s">
         <v>219</v>
-      </c>
-      <c r="D90" t="s">
-        <v>220</v>
       </c>
       <c r="E90">
         <v>20</v>
@@ -3869,13 +3866,13 @@
         <v>8809659047549</v>
       </c>
       <c r="B91" t="s">
+        <v>220</v>
+      </c>
+      <c r="C91" t="s">
         <v>221</v>
       </c>
-      <c r="C91" t="s">
-        <v>222</v>
-      </c>
       <c r="D91" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E91">
         <v>50</v>
@@ -3886,10 +3883,10 @@
         <v>8809659047600</v>
       </c>
       <c r="B92" t="s">
+        <v>222</v>
+      </c>
+      <c r="C92" t="s">
         <v>223</v>
-      </c>
-      <c r="C92" t="s">
-        <v>224</v>
       </c>
       <c r="D92" t="s">
         <v>45</v>
@@ -3903,10 +3900,10 @@
         <v>8809659047631</v>
       </c>
       <c r="B93" t="s">
+        <v>224</v>
+      </c>
+      <c r="C93" t="s">
         <v>225</v>
-      </c>
-      <c r="C93" t="s">
-        <v>226</v>
       </c>
       <c r="D93" t="s">
         <v>42</v>
@@ -3920,13 +3917,13 @@
         <v>8809659047662</v>
       </c>
       <c r="B94" t="s">
+        <v>226</v>
+      </c>
+      <c r="C94" t="s">
         <v>227</v>
       </c>
-      <c r="C94" t="s">
-        <v>228</v>
-      </c>
       <c r="D94" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E94">
         <v>30</v>
@@ -3937,16 +3934,16 @@
         <v>8809659047747</v>
       </c>
       <c r="B95" t="s">
+        <v>228</v>
+      </c>
+      <c r="C95" t="s">
         <v>229</v>
-      </c>
-      <c r="C95" t="s">
-        <v>230</v>
       </c>
       <c r="D95" t="s">
         <v>53</v>
       </c>
       <c r="E95">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="96" spans="1:5">
@@ -3954,16 +3951,16 @@
         <v>8809659047778</v>
       </c>
       <c r="B96" t="s">
+        <v>230</v>
+      </c>
+      <c r="C96" t="s">
         <v>231</v>
-      </c>
-      <c r="C96" t="s">
-        <v>232</v>
       </c>
       <c r="D96" t="s">
         <v>32</v>
       </c>
       <c r="E96">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="97" spans="1:5">
@@ -3971,10 +3968,10 @@
         <v>8809659047884</v>
       </c>
       <c r="B97" t="s">
+        <v>232</v>
+      </c>
+      <c r="C97" t="s">
         <v>233</v>
-      </c>
-      <c r="C97" t="s">
-        <v>234</v>
       </c>
       <c r="D97" t="s">
         <v>45</v>
@@ -3988,16 +3985,16 @@
         <v>8809659048027</v>
       </c>
       <c r="B98" t="s">
+        <v>234</v>
+      </c>
+      <c r="C98" t="s">
         <v>235</v>
-      </c>
-      <c r="C98" t="s">
-        <v>236</v>
       </c>
       <c r="D98" t="s">
         <v>42</v>
       </c>
       <c r="E98">
-        <v>7</v>
+        <v>35</v>
       </c>
     </row>
     <row r="99" spans="1:5">
@@ -4005,13 +4002,13 @@
         <v>8809659048263</v>
       </c>
       <c r="B99" t="s">
+        <v>236</v>
+      </c>
+      <c r="C99" t="s">
         <v>237</v>
       </c>
-      <c r="C99" t="s">
-        <v>238</v>
-      </c>
       <c r="D99" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E99">
         <v>19</v>
@@ -4022,13 +4019,13 @@
         <v>8809659048348</v>
       </c>
       <c r="B100" t="s">
+        <v>238</v>
+      </c>
+      <c r="C100" t="s">
         <v>239</v>
       </c>
-      <c r="C100" t="s">
-        <v>240</v>
-      </c>
       <c r="D100" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E100">
         <v>44</v>
@@ -4039,13 +4036,13 @@
         <v>8809659048379</v>
       </c>
       <c r="B101" t="s">
+        <v>240</v>
+      </c>
+      <c r="C101" t="s">
         <v>241</v>
       </c>
-      <c r="C101" t="s">
-        <v>242</v>
-      </c>
       <c r="D101" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E101">
         <v>35</v>
@@ -4056,16 +4053,16 @@
         <v>8809659048409</v>
       </c>
       <c r="B102" t="s">
+        <v>242</v>
+      </c>
+      <c r="C102" t="s">
         <v>243</v>
       </c>
-      <c r="C102" t="s">
+      <c r="D102" t="s">
         <v>244</v>
       </c>
-      <c r="D102" t="s">
-        <v>245</v>
-      </c>
       <c r="E102">
-        <v>17</v>
+        <v>20</v>
       </c>
     </row>
     <row r="103" spans="1:5">
@@ -4073,13 +4070,13 @@
         <v>8809659048553</v>
       </c>
       <c r="B103" t="s">
+        <v>245</v>
+      </c>
+      <c r="C103" t="s">
         <v>246</v>
       </c>
-      <c r="C103" t="s">
-        <v>247</v>
-      </c>
       <c r="D103" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E103">
         <v>25</v>
@@ -4090,16 +4087,16 @@
         <v>8809659048591</v>
       </c>
       <c r="B104" t="s">
+        <v>247</v>
+      </c>
+      <c r="C104" t="s">
         <v>248</v>
-      </c>
-      <c r="C104" t="s">
-        <v>249</v>
       </c>
       <c r="D104" t="s">
         <v>71</v>
       </c>
       <c r="E104">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="105" spans="1:5">
@@ -4107,10 +4104,10 @@
         <v>8809659048607</v>
       </c>
       <c r="B105" t="s">
+        <v>249</v>
+      </c>
+      <c r="C105" t="s">
         <v>250</v>
-      </c>
-      <c r="C105" t="s">
-        <v>251</v>
       </c>
       <c r="D105" t="s">
         <v>29</v>
@@ -4124,10 +4121,10 @@
         <v>8809659048614</v>
       </c>
       <c r="B106" t="s">
+        <v>251</v>
+      </c>
+      <c r="C106" t="s">
         <v>252</v>
-      </c>
-      <c r="C106" t="s">
-        <v>253</v>
       </c>
       <c r="D106" t="s">
         <v>48</v>
@@ -4141,10 +4138,10 @@
         <v>8809659048621</v>
       </c>
       <c r="B107" t="s">
+        <v>253</v>
+      </c>
+      <c r="C107" t="s">
         <v>254</v>
-      </c>
-      <c r="C107" t="s">
-        <v>255</v>
       </c>
       <c r="D107" t="s">
         <v>71</v>
@@ -4158,16 +4155,16 @@
         <v>8809659048638</v>
       </c>
       <c r="B108" t="s">
+        <v>255</v>
+      </c>
+      <c r="C108" t="s">
         <v>256</v>
       </c>
-      <c r="C108" t="s">
-        <v>257</v>
-      </c>
       <c r="D108" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E108">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="109" spans="1:5">
@@ -4175,13 +4172,13 @@
         <v>8809659048652</v>
       </c>
       <c r="B109" t="s">
+        <v>257</v>
+      </c>
+      <c r="C109" t="s">
         <v>258</v>
       </c>
-      <c r="C109" t="s">
+      <c r="D109" t="s">
         <v>259</v>
-      </c>
-      <c r="D109" t="s">
-        <v>260</v>
       </c>
       <c r="E109">
         <v>16</v>
@@ -4192,10 +4189,10 @@
         <v>8809659048669</v>
       </c>
       <c r="B110" t="s">
+        <v>260</v>
+      </c>
+      <c r="C110" t="s">
         <v>261</v>
-      </c>
-      <c r="C110" t="s">
-        <v>262</v>
       </c>
       <c r="D110" t="s">
         <v>40</v>
@@ -4209,16 +4206,16 @@
         <v>8809659049901</v>
       </c>
       <c r="B111" t="s">
+        <v>262</v>
+      </c>
+      <c r="C111" t="s">
         <v>263</v>
       </c>
-      <c r="C111" t="s">
-        <v>264</v>
-      </c>
       <c r="D111" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E111">
-        <v>3</v>
+        <v>20</v>
       </c>
     </row>
     <row r="112" spans="1:5">
@@ -4226,10 +4223,10 @@
         <v>8809659049987</v>
       </c>
       <c r="B112" t="s">
+        <v>264</v>
+      </c>
+      <c r="C112" t="s">
         <v>265</v>
-      </c>
-      <c r="C112" t="s">
-        <v>266</v>
       </c>
       <c r="D112" t="s">
         <v>53</v>
@@ -4243,10 +4240,10 @@
         <v>8809671010248</v>
       </c>
       <c r="B113" t="s">
+        <v>266</v>
+      </c>
+      <c r="C113" t="s">
         <v>267</v>
-      </c>
-      <c r="C113" t="s">
-        <v>268</v>
       </c>
       <c r="D113" t="s">
         <v>65</v>
@@ -4260,13 +4257,13 @@
         <v>8809671010293</v>
       </c>
       <c r="B114" t="s">
+        <v>268</v>
+      </c>
+      <c r="C114" t="s">
         <v>269</v>
       </c>
-      <c r="C114" t="s">
+      <c r="D114" t="s">
         <v>270</v>
-      </c>
-      <c r="D114" t="s">
-        <v>271</v>
       </c>
       <c r="E114">
         <v>10</v>
@@ -4277,10 +4274,10 @@
         <v>8809685620754</v>
       </c>
       <c r="B115" t="s">
+        <v>271</v>
+      </c>
+      <c r="C115" t="s">
         <v>272</v>
-      </c>
-      <c r="C115" t="s">
-        <v>273</v>
       </c>
       <c r="D115" t="s">
         <v>65</v>
@@ -4294,16 +4291,16 @@
         <v>8809685622932</v>
       </c>
       <c r="B116" t="s">
+        <v>273</v>
+      </c>
+      <c r="C116" t="s">
         <v>274</v>
       </c>
-      <c r="C116" t="s">
-        <v>275</v>
-      </c>
       <c r="D116" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E116">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="117" spans="1:5">
@@ -4311,16 +4308,16 @@
         <v>8809685623991</v>
       </c>
       <c r="B117" t="s">
+        <v>275</v>
+      </c>
+      <c r="C117" t="s">
         <v>276</v>
       </c>
-      <c r="C117" t="s">
-        <v>277</v>
-      </c>
       <c r="D117" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E117">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="118" spans="1:5">
@@ -4328,13 +4325,13 @@
         <v>8809685624028</v>
       </c>
       <c r="B118" t="s">
+        <v>277</v>
+      </c>
+      <c r="C118" t="s">
         <v>278</v>
       </c>
-      <c r="C118" t="s">
-        <v>279</v>
-      </c>
       <c r="D118" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E118">
         <v>50</v>
@@ -4345,13 +4342,13 @@
         <v>8809685624035</v>
       </c>
       <c r="B119" t="s">
+        <v>279</v>
+      </c>
+      <c r="C119" t="s">
         <v>280</v>
       </c>
-      <c r="C119" t="s">
-        <v>281</v>
-      </c>
       <c r="D119" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E119">
         <v>18</v>
@@ -4362,13 +4359,13 @@
         <v>8809685624042</v>
       </c>
       <c r="B120" t="s">
+        <v>281</v>
+      </c>
+      <c r="C120" t="s">
         <v>282</v>
       </c>
-      <c r="C120" t="s">
-        <v>283</v>
-      </c>
       <c r="D120" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E120">
         <v>16</v>
@@ -4379,13 +4376,13 @@
         <v>8809685624660</v>
       </c>
       <c r="B121" t="s">
+        <v>283</v>
+      </c>
+      <c r="C121" t="s">
         <v>284</v>
       </c>
-      <c r="C121" t="s">
-        <v>285</v>
-      </c>
       <c r="D121" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E121">
         <v>42</v>
@@ -4396,10 +4393,10 @@
         <v>8809685624721</v>
       </c>
       <c r="B122" t="s">
+        <v>285</v>
+      </c>
+      <c r="C122" t="s">
         <v>286</v>
-      </c>
-      <c r="C122" t="s">
-        <v>287</v>
       </c>
       <c r="D122" t="s">
         <v>65</v>
@@ -4413,16 +4410,16 @@
         <v>8809685624745</v>
       </c>
       <c r="B123" t="s">
+        <v>287</v>
+      </c>
+      <c r="C123" t="s">
         <v>288</v>
       </c>
-      <c r="C123" t="s">
-        <v>289</v>
-      </c>
       <c r="D123" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E123">
-        <v>9</v>
+        <v>20</v>
       </c>
     </row>
     <row r="124" spans="1:5">
@@ -4430,10 +4427,10 @@
         <v>8809685625001</v>
       </c>
       <c r="B124" t="s">
+        <v>289</v>
+      </c>
+      <c r="C124" t="s">
         <v>290</v>
-      </c>
-      <c r="C124" t="s">
-        <v>291</v>
       </c>
       <c r="D124" t="s">
         <v>32</v>
@@ -4447,10 +4444,10 @@
         <v>8809685625469</v>
       </c>
       <c r="B125" t="s">
+        <v>291</v>
+      </c>
+      <c r="C125" t="s">
         <v>292</v>
-      </c>
-      <c r="C125" t="s">
-        <v>293</v>
       </c>
       <c r="D125" t="s">
         <v>40</v>
@@ -4464,13 +4461,13 @@
         <v>8809685625759</v>
       </c>
       <c r="B126" t="s">
+        <v>293</v>
+      </c>
+      <c r="C126" t="s">
         <v>294</v>
       </c>
-      <c r="C126" t="s">
+      <c r="D126" t="s">
         <v>295</v>
-      </c>
-      <c r="D126" t="s">
-        <v>296</v>
       </c>
       <c r="E126">
         <v>30</v>
@@ -4481,13 +4478,13 @@
         <v>8809685626176</v>
       </c>
       <c r="B127" t="s">
+        <v>296</v>
+      </c>
+      <c r="C127" t="s">
         <v>297</v>
       </c>
-      <c r="C127" t="s">
-        <v>298</v>
-      </c>
       <c r="D127" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E127">
         <v>37</v>
@@ -4498,16 +4495,16 @@
         <v>8809685626558</v>
       </c>
       <c r="B128" t="s">
+        <v>298</v>
+      </c>
+      <c r="C128" t="s">
         <v>299</v>
-      </c>
-      <c r="C128" t="s">
-        <v>300</v>
       </c>
       <c r="D128" t="s">
         <v>35</v>
       </c>
       <c r="E128">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="129" spans="1:5">
@@ -4515,16 +4512,16 @@
         <v>8809685627067</v>
       </c>
       <c r="B129" t="s">
+        <v>300</v>
+      </c>
+      <c r="C129" t="s">
         <v>301</v>
       </c>
-      <c r="C129" t="s">
-        <v>302</v>
-      </c>
       <c r="D129" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E129">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="130" spans="1:5">
@@ -4532,16 +4529,16 @@
         <v>8809685627081</v>
       </c>
       <c r="B130" t="s">
+        <v>302</v>
+      </c>
+      <c r="C130" t="s">
         <v>303</v>
       </c>
-      <c r="C130" t="s">
-        <v>304</v>
-      </c>
       <c r="D130" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E130">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="131" spans="1:5">
@@ -4549,16 +4546,16 @@
         <v>8809685629344</v>
       </c>
       <c r="B131" t="s">
+        <v>304</v>
+      </c>
+      <c r="C131" t="s">
         <v>305</v>
-      </c>
-      <c r="C131" t="s">
-        <v>306</v>
       </c>
       <c r="D131" t="s">
         <v>24</v>
       </c>
       <c r="E131">
-        <v>11</v>
+        <v>20</v>
       </c>
     </row>
     <row r="132" spans="1:5">
@@ -4566,13 +4563,13 @@
         <v>8809688890093</v>
       </c>
       <c r="B132" t="s">
+        <v>306</v>
+      </c>
+      <c r="C132" t="s">
         <v>307</v>
       </c>
-      <c r="C132" t="s">
-        <v>308</v>
-      </c>
       <c r="D132" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E132">
         <v>39</v>
@@ -4583,16 +4580,16 @@
         <v>8809688890123</v>
       </c>
       <c r="B133" t="s">
+        <v>308</v>
+      </c>
+      <c r="C133" t="s">
         <v>309</v>
       </c>
-      <c r="C133" t="s">
-        <v>310</v>
-      </c>
       <c r="D133" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E133">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="134" spans="1:5">
@@ -4600,16 +4597,16 @@
         <v>8809688891106</v>
       </c>
       <c r="B134" t="s">
+        <v>310</v>
+      </c>
+      <c r="C134" t="s">
         <v>311</v>
       </c>
-      <c r="C134" t="s">
-        <v>312</v>
-      </c>
       <c r="D134" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E134">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="135" spans="1:5">
@@ -4617,13 +4614,13 @@
         <v>8809688891137</v>
       </c>
       <c r="B135" t="s">
+        <v>312</v>
+      </c>
+      <c r="C135" t="s">
         <v>313</v>
       </c>
-      <c r="C135" t="s">
-        <v>314</v>
-      </c>
       <c r="D135" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E135">
         <v>44</v>
@@ -4634,10 +4631,10 @@
         <v>8809688891229</v>
       </c>
       <c r="B136" t="s">
+        <v>314</v>
+      </c>
+      <c r="C136" t="s">
         <v>315</v>
-      </c>
-      <c r="C136" t="s">
-        <v>316</v>
       </c>
       <c r="D136" t="s">
         <v>53</v>
@@ -4651,16 +4648,16 @@
         <v>8809688891557</v>
       </c>
       <c r="B137" t="s">
+        <v>316</v>
+      </c>
+      <c r="C137" t="s">
         <v>317</v>
       </c>
-      <c r="C137" t="s">
-        <v>318</v>
-      </c>
       <c r="D137" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E137">
-        <v>14</v>
+        <v>16</v>
       </c>
     </row>
     <row r="138" spans="1:5">
@@ -4668,16 +4665,16 @@
         <v>8809688891977</v>
       </c>
       <c r="B138" t="s">
+        <v>318</v>
+      </c>
+      <c r="C138" t="s">
         <v>319</v>
-      </c>
-      <c r="C138" t="s">
-        <v>320</v>
       </c>
       <c r="D138" t="s">
         <v>32</v>
       </c>
       <c r="E138">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="139" spans="1:5">
@@ -4685,13 +4682,13 @@
         <v>8809688892066</v>
       </c>
       <c r="B139" t="s">
+        <v>320</v>
+      </c>
+      <c r="C139" t="s">
         <v>321</v>
       </c>
-      <c r="C139" t="s">
-        <v>322</v>
-      </c>
       <c r="D139" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E139">
         <v>20</v>
@@ -4702,16 +4699,16 @@
         <v>8809688892295</v>
       </c>
       <c r="B140" t="s">
+        <v>322</v>
+      </c>
+      <c r="C140" t="s">
         <v>323</v>
       </c>
-      <c r="C140" t="s">
-        <v>324</v>
-      </c>
       <c r="D140" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E140">
-        <v>36</v>
+        <v>40</v>
       </c>
     </row>
     <row r="141" spans="1:5">
@@ -4719,13 +4716,13 @@
         <v>8809688893018</v>
       </c>
       <c r="B141" t="s">
+        <v>324</v>
+      </c>
+      <c r="C141" t="s">
         <v>325</v>
       </c>
-      <c r="C141" t="s">
-        <v>326</v>
-      </c>
       <c r="D141" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E141">
         <v>15</v>
@@ -4736,16 +4733,16 @@
         <v>8809688893049</v>
       </c>
       <c r="B142" t="s">
+        <v>326</v>
+      </c>
+      <c r="C142" t="s">
         <v>327</v>
       </c>
-      <c r="C142" t="s">
-        <v>328</v>
-      </c>
       <c r="D142" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E142">
-        <v>5</v>
+        <v>15</v>
       </c>
     </row>
     <row r="143" spans="1:5">
@@ -4753,13 +4750,13 @@
         <v>8809688893070</v>
       </c>
       <c r="B143" t="s">
+        <v>328</v>
+      </c>
+      <c r="C143" t="s">
         <v>329</v>
       </c>
-      <c r="C143" t="s">
-        <v>330</v>
-      </c>
       <c r="D143" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E143">
         <v>42</v>
@@ -4770,13 +4767,13 @@
         <v>8809688893100</v>
       </c>
       <c r="B144" t="s">
+        <v>330</v>
+      </c>
+      <c r="C144" t="s">
         <v>331</v>
       </c>
-      <c r="C144" t="s">
-        <v>332</v>
-      </c>
       <c r="D144" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E144">
         <v>20</v>
@@ -4787,13 +4784,13 @@
         <v>8809688893131</v>
       </c>
       <c r="B145" t="s">
+        <v>332</v>
+      </c>
+      <c r="C145" t="s">
         <v>333</v>
       </c>
-      <c r="C145" t="s">
+      <c r="D145" t="s">
         <v>334</v>
-      </c>
-      <c r="D145" t="s">
-        <v>335</v>
       </c>
       <c r="E145">
         <v>20</v>
@@ -4804,10 +4801,10 @@
         <v>8809688893162</v>
       </c>
       <c r="B146" t="s">
+        <v>335</v>
+      </c>
+      <c r="C146" t="s">
         <v>336</v>
-      </c>
-      <c r="C146" t="s">
-        <v>337</v>
       </c>
       <c r="D146" t="s">
         <v>45</v>
@@ -4821,10 +4818,10 @@
         <v>8809688893193</v>
       </c>
       <c r="B147" t="s">
+        <v>337</v>
+      </c>
+      <c r="C147" t="s">
         <v>338</v>
-      </c>
-      <c r="C147" t="s">
-        <v>339</v>
       </c>
       <c r="D147" t="s">
         <v>95</v>
@@ -4838,16 +4835,16 @@
         <v>8809688893513</v>
       </c>
       <c r="B148" t="s">
+        <v>339</v>
+      </c>
+      <c r="C148" t="s">
         <v>340</v>
       </c>
-      <c r="C148" t="s">
-        <v>341</v>
-      </c>
       <c r="D148" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E148">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="149" spans="1:5">
@@ -4855,16 +4852,16 @@
         <v>8809688893568</v>
       </c>
       <c r="B149" t="s">
+        <v>341</v>
+      </c>
+      <c r="C149" t="s">
         <v>342</v>
       </c>
-      <c r="C149" t="s">
-        <v>343</v>
-      </c>
       <c r="D149" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E149">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="150" spans="1:5">
@@ -4872,16 +4869,16 @@
         <v>8809688893698</v>
       </c>
       <c r="B150" t="s">
+        <v>343</v>
+      </c>
+      <c r="C150" t="s">
         <v>344</v>
-      </c>
-      <c r="C150" t="s">
-        <v>345</v>
       </c>
       <c r="D150" t="s">
         <v>42</v>
       </c>
       <c r="E150">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="151" spans="1:5">
@@ -4889,16 +4886,16 @@
         <v>8809688893728</v>
       </c>
       <c r="B151" t="s">
+        <v>345</v>
+      </c>
+      <c r="C151" t="s">
         <v>346</v>
       </c>
-      <c r="C151" t="s">
-        <v>347</v>
-      </c>
       <c r="D151" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E151">
-        <v>15</v>
+        <v>19</v>
       </c>
     </row>
     <row r="152" spans="1:5">
@@ -4906,16 +4903,16 @@
         <v>8809688893759</v>
       </c>
       <c r="B152" t="s">
+        <v>347</v>
+      </c>
+      <c r="C152" t="s">
         <v>348</v>
       </c>
-      <c r="C152" t="s">
-        <v>349</v>
-      </c>
       <c r="D152" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E152">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="153" spans="1:5">
@@ -4923,13 +4920,13 @@
         <v>8809688893780</v>
       </c>
       <c r="B153" t="s">
+        <v>349</v>
+      </c>
+      <c r="C153" t="s">
         <v>350</v>
       </c>
-      <c r="C153" t="s">
-        <v>351</v>
-      </c>
       <c r="D153" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E153">
         <v>30</v>
@@ -4940,13 +4937,13 @@
         <v>8809688894046</v>
       </c>
       <c r="B154" t="s">
+        <v>351</v>
+      </c>
+      <c r="C154" t="s">
         <v>352</v>
       </c>
-      <c r="C154" t="s">
-        <v>353</v>
-      </c>
       <c r="D154" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E154">
         <v>21</v>
@@ -4957,13 +4954,13 @@
         <v>8809688894077</v>
       </c>
       <c r="B155" t="s">
+        <v>353</v>
+      </c>
+      <c r="C155" t="s">
         <v>354</v>
       </c>
-      <c r="C155" t="s">
-        <v>355</v>
-      </c>
       <c r="D155" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E155">
         <v>40</v>
@@ -4974,13 +4971,13 @@
         <v>8809688894107</v>
       </c>
       <c r="B156" t="s">
+        <v>355</v>
+      </c>
+      <c r="C156" t="s">
         <v>356</v>
       </c>
-      <c r="C156" t="s">
-        <v>357</v>
-      </c>
       <c r="D156" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E156">
         <v>20</v>
@@ -4991,16 +4988,16 @@
         <v>8809688894138</v>
       </c>
       <c r="B157" t="s">
+        <v>357</v>
+      </c>
+      <c r="C157" t="s">
         <v>358</v>
       </c>
-      <c r="C157" t="s">
-        <v>359</v>
-      </c>
       <c r="D157" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E157">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="158" spans="1:5">
@@ -5008,10 +5005,10 @@
         <v>8809688894152</v>
       </c>
       <c r="B158" t="s">
+        <v>359</v>
+      </c>
+      <c r="C158" t="s">
         <v>360</v>
-      </c>
-      <c r="C158" t="s">
-        <v>361</v>
       </c>
       <c r="D158" t="s">
         <v>68</v>
@@ -5025,13 +5022,13 @@
         <v>8809688894183</v>
       </c>
       <c r="B159" t="s">
+        <v>361</v>
+      </c>
+      <c r="C159" t="s">
         <v>362</v>
       </c>
-      <c r="C159" t="s">
-        <v>363</v>
-      </c>
       <c r="D159" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="E159">
         <v>19</v>
@@ -5042,10 +5039,10 @@
         <v>8809688894213</v>
       </c>
       <c r="B160" t="s">
+        <v>363</v>
+      </c>
+      <c r="C160" t="s">
         <v>364</v>
-      </c>
-      <c r="C160" t="s">
-        <v>365</v>
       </c>
       <c r="D160" t="s">
         <v>29</v>
@@ -5059,10 +5056,10 @@
         <v>8809688894244</v>
       </c>
       <c r="B161" t="s">
+        <v>365</v>
+      </c>
+      <c r="C161" t="s">
         <v>366</v>
-      </c>
-      <c r="C161" t="s">
-        <v>367</v>
       </c>
       <c r="D161" t="s">
         <v>24</v>
@@ -5076,13 +5073,13 @@
         <v>8809688894466</v>
       </c>
       <c r="B162" t="s">
+        <v>367</v>
+      </c>
+      <c r="C162" t="s">
         <v>368</v>
       </c>
-      <c r="C162" t="s">
-        <v>369</v>
-      </c>
       <c r="D162" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E162">
         <v>11</v>
@@ -5093,13 +5090,13 @@
         <v>8809688894558</v>
       </c>
       <c r="B163" t="s">
+        <v>369</v>
+      </c>
+      <c r="C163" t="s">
         <v>370</v>
       </c>
-      <c r="C163" t="s">
-        <v>371</v>
-      </c>
       <c r="D163" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E163">
         <v>18</v>
@@ -5110,16 +5107,16 @@
         <v>8809688894640</v>
       </c>
       <c r="B164" t="s">
+        <v>371</v>
+      </c>
+      <c r="C164" t="s">
         <v>372</v>
       </c>
-      <c r="C164" t="s">
-        <v>373</v>
-      </c>
       <c r="D164" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E164">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="165" spans="1:5">
@@ -5127,16 +5124,16 @@
         <v>8809688895388</v>
       </c>
       <c r="B165" t="s">
+        <v>373</v>
+      </c>
+      <c r="C165" t="s">
         <v>374</v>
       </c>
-      <c r="C165" t="s">
-        <v>375</v>
-      </c>
       <c r="D165" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E165">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="166" spans="1:5">
@@ -5144,13 +5141,13 @@
         <v>8809688896583</v>
       </c>
       <c r="B166" t="s">
+        <v>375</v>
+      </c>
+      <c r="C166" t="s">
         <v>376</v>
       </c>
-      <c r="C166" t="s">
-        <v>377</v>
-      </c>
       <c r="D166" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E166">
         <v>32</v>
@@ -5161,13 +5158,13 @@
         <v>8809688896590</v>
       </c>
       <c r="B167" t="s">
+        <v>377</v>
+      </c>
+      <c r="C167" t="s">
         <v>378</v>
       </c>
-      <c r="C167" t="s">
-        <v>379</v>
-      </c>
       <c r="D167" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E167">
         <v>15</v>
@@ -5178,10 +5175,10 @@
         <v>8809688896606</v>
       </c>
       <c r="B168" t="s">
+        <v>379</v>
+      </c>
+      <c r="C168" t="s">
         <v>380</v>
-      </c>
-      <c r="C168" t="s">
-        <v>381</v>
       </c>
       <c r="D168" t="s">
         <v>90</v>
@@ -5195,13 +5192,13 @@
         <v>8809688896613</v>
       </c>
       <c r="B169" t="s">
+        <v>381</v>
+      </c>
+      <c r="C169" t="s">
         <v>382</v>
       </c>
-      <c r="C169" t="s">
-        <v>383</v>
-      </c>
       <c r="D169" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="E169">
         <v>13</v>
@@ -5212,10 +5209,10 @@
         <v>8809688896620</v>
       </c>
       <c r="B170" t="s">
+        <v>383</v>
+      </c>
+      <c r="C170" t="s">
         <v>384</v>
-      </c>
-      <c r="C170" t="s">
-        <v>385</v>
       </c>
       <c r="D170" t="s">
         <v>32</v>
@@ -5229,10 +5226,10 @@
         <v>8809688896637</v>
       </c>
       <c r="B171" t="s">
+        <v>385</v>
+      </c>
+      <c r="C171" t="s">
         <v>386</v>
-      </c>
-      <c r="C171" t="s">
-        <v>387</v>
       </c>
       <c r="D171" t="s">
         <v>48</v>
@@ -5246,13 +5243,13 @@
         <v>8809688896644</v>
       </c>
       <c r="B172" t="s">
+        <v>387</v>
+      </c>
+      <c r="C172" t="s">
         <v>388</v>
       </c>
-      <c r="C172" t="s">
+      <c r="D172" t="s">
         <v>389</v>
-      </c>
-      <c r="D172" t="s">
-        <v>390</v>
       </c>
       <c r="E172">
         <v>30</v>
@@ -5263,13 +5260,13 @@
         <v>8809688896675</v>
       </c>
       <c r="B173" t="s">
+        <v>390</v>
+      </c>
+      <c r="C173" t="s">
         <v>391</v>
       </c>
-      <c r="C173" t="s">
+      <c r="D173" t="s">
         <v>392</v>
-      </c>
-      <c r="D173" t="s">
-        <v>393</v>
       </c>
       <c r="E173">
         <v>15</v>
@@ -5280,13 +5277,13 @@
         <v>8809688896736</v>
       </c>
       <c r="B174" t="s">
+        <v>393</v>
+      </c>
+      <c r="C174" t="s">
         <v>394</v>
       </c>
-      <c r="C174" t="s">
-        <v>395</v>
-      </c>
       <c r="D174" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E174">
         <v>28</v>
@@ -5297,13 +5294,13 @@
         <v>8809688896804</v>
       </c>
       <c r="B175" t="s">
+        <v>395</v>
+      </c>
+      <c r="C175" t="s">
         <v>396</v>
       </c>
-      <c r="C175" t="s">
-        <v>397</v>
-      </c>
       <c r="D175" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E175">
         <v>50</v>
@@ -5314,16 +5311,16 @@
         <v>8809688896835</v>
       </c>
       <c r="B176" t="s">
+        <v>397</v>
+      </c>
+      <c r="C176" t="s">
         <v>398</v>
       </c>
-      <c r="C176" t="s">
-        <v>399</v>
-      </c>
       <c r="D176" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E176">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="177" spans="1:5">
@@ -5331,13 +5328,13 @@
         <v>8809688896866</v>
       </c>
       <c r="B177" t="s">
+        <v>399</v>
+      </c>
+      <c r="C177" t="s">
         <v>400</v>
       </c>
-      <c r="C177" t="s">
-        <v>401</v>
-      </c>
       <c r="D177" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E177">
         <v>19</v>
@@ -5348,13 +5345,13 @@
         <v>8809688896897</v>
       </c>
       <c r="B178" t="s">
+        <v>401</v>
+      </c>
+      <c r="C178" t="s">
         <v>402</v>
       </c>
-      <c r="C178" t="s">
-        <v>403</v>
-      </c>
       <c r="D178" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E178">
         <v>20</v>
@@ -5365,13 +5362,13 @@
         <v>8809688896910</v>
       </c>
       <c r="B179" t="s">
+        <v>403</v>
+      </c>
+      <c r="C179" t="s">
         <v>404</v>
       </c>
-      <c r="C179" t="s">
+      <c r="D179" t="s">
         <v>405</v>
-      </c>
-      <c r="D179" t="s">
-        <v>406</v>
       </c>
       <c r="E179">
         <v>50</v>
@@ -5382,13 +5379,13 @@
         <v>8809688896941</v>
       </c>
       <c r="B180" t="s">
+        <v>406</v>
+      </c>
+      <c r="C180" t="s">
         <v>407</v>
       </c>
-      <c r="C180" t="s">
-        <v>408</v>
-      </c>
       <c r="D180" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E180">
         <v>16</v>
@@ -5399,10 +5396,10 @@
         <v>8809688896972</v>
       </c>
       <c r="B181" t="s">
+        <v>408</v>
+      </c>
+      <c r="C181" t="s">
         <v>409</v>
-      </c>
-      <c r="C181" t="s">
-        <v>410</v>
       </c>
       <c r="D181" t="s">
         <v>53</v>
@@ -5416,16 +5413,16 @@
         <v>8809688897009</v>
       </c>
       <c r="B182" t="s">
+        <v>410</v>
+      </c>
+      <c r="C182" t="s">
         <v>411</v>
-      </c>
-      <c r="C182" t="s">
-        <v>412</v>
       </c>
       <c r="D182" t="s">
         <v>68</v>
       </c>
       <c r="E182">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="183" spans="1:5">
@@ -5433,10 +5430,10 @@
         <v>8809688897016</v>
       </c>
       <c r="B183" t="s">
+        <v>412</v>
+      </c>
+      <c r="C183" t="s">
         <v>413</v>
-      </c>
-      <c r="C183" t="s">
-        <v>414</v>
       </c>
       <c r="D183" t="s">
         <v>32</v>
@@ -5450,16 +5447,16 @@
         <v>8809688897344</v>
       </c>
       <c r="B184" t="s">
+        <v>414</v>
+      </c>
+      <c r="C184" t="s">
         <v>415</v>
       </c>
-      <c r="C184" t="s">
-        <v>416</v>
-      </c>
       <c r="D184" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E184">
-        <v>8</v>
+        <v>30</v>
       </c>
     </row>
     <row r="185" spans="1:5">
@@ -5467,13 +5464,13 @@
         <v>8809688897368</v>
       </c>
       <c r="B185" t="s">
+        <v>416</v>
+      </c>
+      <c r="C185" t="s">
         <v>417</v>
       </c>
-      <c r="C185" t="s">
-        <v>418</v>
-      </c>
       <c r="D185" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E185">
         <v>15</v>
@@ -5484,16 +5481,16 @@
         <v>8809688897382</v>
       </c>
       <c r="B186" t="s">
+        <v>418</v>
+      </c>
+      <c r="C186" t="s">
         <v>419</v>
-      </c>
-      <c r="C186" t="s">
-        <v>420</v>
       </c>
       <c r="D186" t="s">
         <v>56</v>
       </c>
       <c r="E186">
-        <v>6</v>
+        <v>10</v>
       </c>
     </row>
     <row r="187" spans="1:5">
@@ -5501,16 +5498,16 @@
         <v>8809688897412</v>
       </c>
       <c r="B187" t="s">
+        <v>420</v>
+      </c>
+      <c r="C187" t="s">
         <v>421</v>
       </c>
-      <c r="C187" t="s">
-        <v>422</v>
-      </c>
       <c r="D187" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E187">
-        <v>4</v>
+        <v>50</v>
       </c>
     </row>
     <row r="188" spans="1:5">
@@ -5518,16 +5515,16 @@
         <v>8809688897504</v>
       </c>
       <c r="B188" t="s">
+        <v>422</v>
+      </c>
+      <c r="C188" t="s">
         <v>423</v>
       </c>
-      <c r="C188" t="s">
-        <v>424</v>
-      </c>
       <c r="D188" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E188">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="189" spans="1:5">
@@ -5535,16 +5532,16 @@
         <v>8809688897535</v>
       </c>
       <c r="B189" t="s">
+        <v>424</v>
+      </c>
+      <c r="C189" t="s">
         <v>425</v>
       </c>
-      <c r="C189" t="s">
-        <v>426</v>
-      </c>
       <c r="D189" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E189">
-        <v>-2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="190" spans="1:5">
@@ -5552,16 +5549,16 @@
         <v>8809688897566</v>
       </c>
       <c r="B190" t="s">
+        <v>426</v>
+      </c>
+      <c r="C190" t="s">
         <v>427</v>
       </c>
-      <c r="C190" t="s">
-        <v>428</v>
-      </c>
       <c r="D190" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E190">
-        <v>16</v>
+        <v>25</v>
       </c>
     </row>
     <row r="191" spans="1:5">
@@ -5569,16 +5566,16 @@
         <v>8809688897658</v>
       </c>
       <c r="B191" t="s">
+        <v>428</v>
+      </c>
+      <c r="C191" t="s">
         <v>429</v>
       </c>
-      <c r="C191" t="s">
-        <v>430</v>
-      </c>
       <c r="D191" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E191">
-        <v>20</v>
+        <v>25</v>
       </c>
     </row>
     <row r="192" spans="1:5">
@@ -5586,16 +5583,16 @@
         <v>8809688897733</v>
       </c>
       <c r="B192" t="s">
+        <v>430</v>
+      </c>
+      <c r="C192" t="s">
         <v>431</v>
       </c>
-      <c r="C192" t="s">
-        <v>432</v>
-      </c>
       <c r="D192" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="E192">
-        <v>13</v>
+        <v>23</v>
       </c>
     </row>
     <row r="193" spans="1:5">
@@ -5603,16 +5600,16 @@
         <v>8809688897764</v>
       </c>
       <c r="B193" t="s">
+        <v>432</v>
+      </c>
+      <c r="C193" t="s">
         <v>433</v>
       </c>
-      <c r="C193" t="s">
-        <v>434</v>
-      </c>
       <c r="D193" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="E193">
-        <v>16</v>
+        <v>18</v>
       </c>
     </row>
     <row r="194" spans="1:5">
@@ -5620,13 +5617,13 @@
         <v>8809688897795</v>
       </c>
       <c r="B194" t="s">
+        <v>434</v>
+      </c>
+      <c r="C194" t="s">
         <v>435</v>
       </c>
-      <c r="C194" t="s">
-        <v>436</v>
-      </c>
       <c r="D194" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E194">
         <v>16</v>
@@ -5637,13 +5634,13 @@
         <v>8809688897887</v>
       </c>
       <c r="B195" t="s">
+        <v>436</v>
+      </c>
+      <c r="C195" t="s">
         <v>437</v>
       </c>
-      <c r="C195" t="s">
-        <v>438</v>
-      </c>
       <c r="D195" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
       <c r="E195">
         <v>20</v>
@@ -5654,16 +5651,16 @@
         <v>8809688897962</v>
       </c>
       <c r="B196" t="s">
+        <v>438</v>
+      </c>
+      <c r="C196" t="s">
         <v>439</v>
       </c>
-      <c r="C196" t="s">
-        <v>440</v>
-      </c>
       <c r="D196" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E196">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="197" spans="1:5">
@@ -5671,16 +5668,16 @@
         <v>8809688897993</v>
       </c>
       <c r="B197" t="s">
+        <v>440</v>
+      </c>
+      <c r="C197" t="s">
         <v>441</v>
-      </c>
-      <c r="C197" t="s">
-        <v>442</v>
       </c>
       <c r="D197" t="s">
         <v>24</v>
       </c>
       <c r="E197">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="198" spans="1:5">
@@ -5688,10 +5685,10 @@
         <v>8809688898020</v>
       </c>
       <c r="B198" t="s">
+        <v>442</v>
+      </c>
+      <c r="C198" t="s">
         <v>443</v>
-      </c>
-      <c r="C198" t="s">
-        <v>444</v>
       </c>
       <c r="D198" t="s">
         <v>90</v>
@@ -5705,13 +5702,13 @@
         <v>8809688898112</v>
       </c>
       <c r="B199" t="s">
+        <v>444</v>
+      </c>
+      <c r="C199" t="s">
         <v>445</v>
       </c>
-      <c r="C199" t="s">
-        <v>446</v>
-      </c>
       <c r="D199" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E199">
         <v>50</v>
@@ -5722,13 +5719,13 @@
         <v>8809688898402</v>
       </c>
       <c r="B200" t="s">
+        <v>446</v>
+      </c>
+      <c r="C200" t="s">
         <v>447</v>
       </c>
-      <c r="C200" t="s">
-        <v>448</v>
-      </c>
       <c r="D200" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E200">
         <v>20</v>
@@ -5739,10 +5736,10 @@
         <v>8809688898433</v>
       </c>
       <c r="B201" t="s">
+        <v>448</v>
+      </c>
+      <c r="C201" t="s">
         <v>449</v>
-      </c>
-      <c r="C201" t="s">
-        <v>450</v>
       </c>
       <c r="D201" t="s">
         <v>74</v>
@@ -5756,10 +5753,10 @@
         <v>8809688898464</v>
       </c>
       <c r="B202" t="s">
+        <v>450</v>
+      </c>
+      <c r="C202" t="s">
         <v>451</v>
-      </c>
-      <c r="C202" t="s">
-        <v>452</v>
       </c>
       <c r="D202" t="s">
         <v>82</v>
@@ -5773,13 +5770,13 @@
         <v>8809688898495</v>
       </c>
       <c r="B203" t="s">
+        <v>452</v>
+      </c>
+      <c r="C203" t="s">
         <v>453</v>
       </c>
-      <c r="C203" t="s">
-        <v>454</v>
-      </c>
       <c r="D203" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E203">
         <v>30</v>
@@ -5790,16 +5787,16 @@
         <v>8809688898525</v>
       </c>
       <c r="B204" t="s">
+        <v>454</v>
+      </c>
+      <c r="C204" t="s">
         <v>455</v>
       </c>
-      <c r="C204" t="s">
-        <v>456</v>
-      </c>
       <c r="D204" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E204">
-        <v>6</v>
+        <v>20</v>
       </c>
     </row>
     <row r="205" spans="1:5">
@@ -5807,10 +5804,10 @@
         <v>8809688899430</v>
       </c>
       <c r="B205" t="s">
+        <v>456</v>
+      </c>
+      <c r="C205" t="s">
         <v>457</v>
-      </c>
-      <c r="C205" t="s">
-        <v>458</v>
       </c>
       <c r="D205" t="s">
         <v>82</v>
@@ -5824,16 +5821,16 @@
         <v>8809688899461</v>
       </c>
       <c r="B206" t="s">
+        <v>458</v>
+      </c>
+      <c r="C206" t="s">
         <v>459</v>
       </c>
-      <c r="C206" t="s">
-        <v>460</v>
-      </c>
       <c r="D206" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="E206">
-        <v>9</v>
+        <v>11</v>
       </c>
     </row>
     <row r="207" spans="1:5">
@@ -5841,13 +5838,13 @@
         <v>8809688899492</v>
       </c>
       <c r="B207" t="s">
+        <v>460</v>
+      </c>
+      <c r="C207" t="s">
         <v>461</v>
       </c>
-      <c r="C207" t="s">
-        <v>462</v>
-      </c>
       <c r="D207" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E207">
         <v>37</v>
@@ -5858,16 +5855,16 @@
         <v>8809688899522</v>
       </c>
       <c r="B208" t="s">
+        <v>462</v>
+      </c>
+      <c r="C208" t="s">
         <v>463</v>
       </c>
-      <c r="C208" t="s">
+      <c r="D208" t="s">
         <v>464</v>
       </c>
-      <c r="D208" t="s">
-        <v>465</v>
-      </c>
       <c r="E208">
-        <v>1</v>
+        <v>20</v>
       </c>
     </row>
     <row r="209" spans="1:5">
@@ -5875,16 +5872,16 @@
         <v>8809688899553</v>
       </c>
       <c r="B209" t="s">
+        <v>465</v>
+      </c>
+      <c r="C209" t="s">
         <v>466</v>
       </c>
-      <c r="C209" t="s">
-        <v>467</v>
-      </c>
       <c r="D209" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E209">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="210" spans="1:5">
@@ -5892,16 +5889,16 @@
         <v>8809688899584</v>
       </c>
       <c r="B210" t="s">
+        <v>467</v>
+      </c>
+      <c r="C210" t="s">
         <v>468</v>
       </c>
-      <c r="C210" t="s">
-        <v>469</v>
-      </c>
       <c r="D210" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E210">
-        <v>2</v>
+        <v>20</v>
       </c>
     </row>
     <row r="211" spans="1:5">
@@ -5909,10 +5906,10 @@
         <v>8809688899669</v>
       </c>
       <c r="B211" t="s">
+        <v>469</v>
+      </c>
+      <c r="C211" t="s">
         <v>470</v>
-      </c>
-      <c r="C211" t="s">
-        <v>471</v>
       </c>
       <c r="D211" t="s">
         <v>87</v>
@@ -5926,16 +5923,16 @@
         <v>8809688899690</v>
       </c>
       <c r="B212" t="s">
+        <v>471</v>
+      </c>
+      <c r="C212" t="s">
         <v>472</v>
-      </c>
-      <c r="C212" t="s">
-        <v>473</v>
       </c>
       <c r="D212" t="s">
         <v>87</v>
       </c>
       <c r="E212">
-        <v>7</v>
+        <v>25</v>
       </c>
     </row>
     <row r="213" spans="1:5">
@@ -5943,16 +5940,16 @@
         <v>8809710751002</v>
       </c>
       <c r="B213" t="s">
+        <v>473</v>
+      </c>
+      <c r="C213" t="s">
         <v>474</v>
       </c>
-      <c r="C213" t="s">
-        <v>475</v>
-      </c>
       <c r="D213" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E213">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="214" spans="1:5">
@@ -5960,13 +5957,13 @@
         <v>8809716070022</v>
       </c>
       <c r="B214" t="s">
+        <v>475</v>
+      </c>
+      <c r="C214" t="s">
         <v>476</v>
       </c>
-      <c r="C214" t="s">
-        <v>477</v>
-      </c>
       <c r="D214" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E214">
         <v>25</v>
@@ -5977,13 +5974,13 @@
         <v>8809716070039</v>
       </c>
       <c r="B215" t="s">
+        <v>477</v>
+      </c>
+      <c r="C215" t="s">
         <v>478</v>
       </c>
-      <c r="C215" t="s">
-        <v>479</v>
-      </c>
       <c r="D215" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E215">
         <v>10</v>
@@ -5994,10 +5991,10 @@
         <v>8809716070046</v>
       </c>
       <c r="B216" t="s">
+        <v>479</v>
+      </c>
+      <c r="C216" t="s">
         <v>480</v>
-      </c>
-      <c r="C216" t="s">
-        <v>481</v>
       </c>
       <c r="D216" t="s">
         <v>53</v>
@@ -6011,16 +6008,16 @@
         <v>8809716070053</v>
       </c>
       <c r="B217" t="s">
+        <v>481</v>
+      </c>
+      <c r="C217" t="s">
         <v>482</v>
       </c>
-      <c r="C217" t="s">
-        <v>483</v>
-      </c>
       <c r="D217" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="E217">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="218" spans="1:5">
@@ -6028,13 +6025,13 @@
         <v>8809716070060</v>
       </c>
       <c r="B218" t="s">
+        <v>483</v>
+      </c>
+      <c r="C218" t="s">
         <v>484</v>
       </c>
-      <c r="C218" t="s">
-        <v>485</v>
-      </c>
       <c r="D218" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E218">
         <v>25</v>
@@ -6045,10 +6042,10 @@
         <v>8809716070503</v>
       </c>
       <c r="B219" t="s">
+        <v>485</v>
+      </c>
+      <c r="C219" t="s">
         <v>486</v>
-      </c>
-      <c r="C219" t="s">
-        <v>487</v>
       </c>
       <c r="D219" t="s">
         <v>29</v>
@@ -6062,10 +6059,10 @@
         <v>8809716070527</v>
       </c>
       <c r="B220" t="s">
+        <v>487</v>
+      </c>
+      <c r="C220" t="s">
         <v>488</v>
-      </c>
-      <c r="C220" t="s">
-        <v>489</v>
       </c>
       <c r="D220" t="s">
         <v>87</v>
@@ -6079,16 +6076,16 @@
         <v>8809716070541</v>
       </c>
       <c r="B221" t="s">
+        <v>489</v>
+      </c>
+      <c r="C221" t="s">
         <v>490</v>
       </c>
-      <c r="C221" t="s">
-        <v>491</v>
-      </c>
       <c r="D221" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E221">
-        <v>8</v>
+        <v>20</v>
       </c>
     </row>
     <row r="222" spans="1:5">
@@ -6096,16 +6093,16 @@
         <v>8809716070565</v>
       </c>
       <c r="B222" t="s">
+        <v>491</v>
+      </c>
+      <c r="C222" t="s">
         <v>492</v>
       </c>
-      <c r="C222" t="s">
-        <v>493</v>
-      </c>
       <c r="D222" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E222">
-        <v>-1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="223" spans="1:5">
@@ -6113,10 +6110,10 @@
         <v>8809716070657</v>
       </c>
       <c r="B223" t="s">
+        <v>493</v>
+      </c>
+      <c r="C223" t="s">
         <v>494</v>
-      </c>
-      <c r="C223" t="s">
-        <v>495</v>
       </c>
       <c r="D223" t="s">
         <v>42</v>
@@ -6130,13 +6127,13 @@
         <v>8809716070671</v>
       </c>
       <c r="B224" t="s">
+        <v>495</v>
+      </c>
+      <c r="C224" t="s">
         <v>496</v>
       </c>
-      <c r="C224" t="s">
+      <c r="D224" t="s">
         <v>497</v>
-      </c>
-      <c r="D224" t="s">
-        <v>498</v>
       </c>
       <c r="E224">
         <v>19</v>
@@ -6147,10 +6144,10 @@
         <v>8809716070909</v>
       </c>
       <c r="B225" t="s">
+        <v>498</v>
+      </c>
+      <c r="C225" t="s">
         <v>499</v>
-      </c>
-      <c r="C225" t="s">
-        <v>500</v>
       </c>
       <c r="D225" t="s">
         <v>74</v>
@@ -6164,10 +6161,10 @@
         <v>8809716070930</v>
       </c>
       <c r="B226" t="s">
+        <v>500</v>
+      </c>
+      <c r="C226" t="s">
         <v>501</v>
-      </c>
-      <c r="C226" t="s">
-        <v>502</v>
       </c>
       <c r="D226" t="s">
         <v>56</v>
@@ -6181,13 +6178,13 @@
         <v>8809716070961</v>
       </c>
       <c r="B227" t="s">
+        <v>502</v>
+      </c>
+      <c r="C227" t="s">
         <v>503</v>
       </c>
-      <c r="C227" t="s">
-        <v>504</v>
-      </c>
       <c r="D227" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="E227">
         <v>30</v>
@@ -6198,16 +6195,16 @@
         <v>8809716071067</v>
       </c>
       <c r="B228" t="s">
+        <v>504</v>
+      </c>
+      <c r="C228" t="s">
         <v>505</v>
       </c>
-      <c r="C228" t="s">
-        <v>506</v>
-      </c>
       <c r="D228" t="s">
-        <v>406</v>
+        <v>405</v>
       </c>
       <c r="E228">
-        <v>5</v>
+        <v>30</v>
       </c>
     </row>
     <row r="229" spans="1:5">
@@ -6215,16 +6212,16 @@
         <v>8809716071098</v>
       </c>
       <c r="B229" t="s">
+        <v>506</v>
+      </c>
+      <c r="C229" t="s">
         <v>507</v>
       </c>
-      <c r="C229" t="s">
-        <v>508</v>
-      </c>
       <c r="D229" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E229">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="230" spans="1:5">
@@ -6232,16 +6229,16 @@
         <v>8809716071128</v>
       </c>
       <c r="B230" t="s">
+        <v>508</v>
+      </c>
+      <c r="C230" t="s">
         <v>509</v>
-      </c>
-      <c r="C230" t="s">
-        <v>510</v>
       </c>
       <c r="D230" t="s">
         <v>95</v>
       </c>
       <c r="E230">
-        <v>4</v>
+        <v>25</v>
       </c>
     </row>
     <row r="231" spans="1:5">
@@ -6249,16 +6246,16 @@
         <v>8809716071159</v>
       </c>
       <c r="B231" t="s">
+        <v>510</v>
+      </c>
+      <c r="C231" t="s">
         <v>511</v>
-      </c>
-      <c r="C231" t="s">
-        <v>512</v>
       </c>
       <c r="D231" t="s">
         <v>56</v>
       </c>
       <c r="E231">
-        <v>6</v>
+        <v>50</v>
       </c>
     </row>
     <row r="232" spans="1:5">
@@ -6266,13 +6263,13 @@
         <v>8809716071289</v>
       </c>
       <c r="B232" t="s">
+        <v>512</v>
+      </c>
+      <c r="C232" t="s">
         <v>513</v>
       </c>
-      <c r="C232" t="s">
-        <v>514</v>
-      </c>
       <c r="D232" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E232">
         <v>20</v>
@@ -6283,10 +6280,10 @@
         <v>8809716071319</v>
       </c>
       <c r="B233" t="s">
+        <v>514</v>
+      </c>
+      <c r="C233" t="s">
         <v>515</v>
-      </c>
-      <c r="C233" t="s">
-        <v>516</v>
       </c>
       <c r="D233" t="s">
         <v>87</v>
@@ -6300,13 +6297,13 @@
         <v>8809716071340</v>
       </c>
       <c r="B234" t="s">
+        <v>516</v>
+      </c>
+      <c r="C234" t="s">
         <v>517</v>
       </c>
-      <c r="C234" t="s">
-        <v>518</v>
-      </c>
       <c r="D234" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E234">
         <v>40</v>
@@ -6317,13 +6314,13 @@
         <v>8809716071371</v>
       </c>
       <c r="B235" t="s">
+        <v>518</v>
+      </c>
+      <c r="C235" t="s">
         <v>519</v>
       </c>
-      <c r="C235" t="s">
-        <v>520</v>
-      </c>
       <c r="D235" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E235">
         <v>50</v>
@@ -6334,10 +6331,10 @@
         <v>8809716071913</v>
       </c>
       <c r="B236" t="s">
+        <v>520</v>
+      </c>
+      <c r="C236" t="s">
         <v>521</v>
-      </c>
-      <c r="C236" t="s">
-        <v>522</v>
       </c>
       <c r="D236" t="s">
         <v>19</v>
@@ -6351,10 +6348,10 @@
         <v>8809716071937</v>
       </c>
       <c r="B237" t="s">
+        <v>522</v>
+      </c>
+      <c r="C237" t="s">
         <v>523</v>
-      </c>
-      <c r="C237" t="s">
-        <v>524</v>
       </c>
       <c r="D237" t="s">
         <v>45</v>
@@ -6368,13 +6365,13 @@
         <v>8809716071951</v>
       </c>
       <c r="B238" t="s">
+        <v>524</v>
+      </c>
+      <c r="C238" t="s">
         <v>525</v>
       </c>
-      <c r="C238" t="s">
-        <v>526</v>
-      </c>
       <c r="D238" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="E238">
         <v>20</v>
@@ -6385,16 +6382,16 @@
         <v>8809716072422</v>
       </c>
       <c r="B239" t="s">
+        <v>526</v>
+      </c>
+      <c r="C239" t="s">
         <v>527</v>
-      </c>
-      <c r="C239" t="s">
-        <v>528</v>
       </c>
       <c r="D239" t="s">
         <v>95</v>
       </c>
       <c r="E239">
-        <v>2</v>
+        <v>35</v>
       </c>
     </row>
     <row r="240" spans="1:5">
@@ -6402,16 +6399,16 @@
         <v>8809716072446</v>
       </c>
       <c r="B240" t="s">
+        <v>528</v>
+      </c>
+      <c r="C240" t="s">
         <v>529</v>
-      </c>
-      <c r="C240" t="s">
-        <v>530</v>
       </c>
       <c r="D240" t="s">
         <v>56</v>
       </c>
       <c r="E240">
-        <v>7</v>
+        <v>30</v>
       </c>
     </row>
     <row r="241" spans="1:5">
@@ -6419,16 +6416,16 @@
         <v>8809716072477</v>
       </c>
       <c r="B241" t="s">
+        <v>530</v>
+      </c>
+      <c r="C241" t="s">
         <v>531</v>
       </c>
-      <c r="C241" t="s">
-        <v>532</v>
-      </c>
       <c r="D241" t="s">
-        <v>192</v>
+        <v>191</v>
       </c>
       <c r="E241">
-        <v>6</v>
+        <v>30</v>
       </c>
     </row>
     <row r="242" spans="1:5">
@@ -6436,13 +6433,13 @@
         <v>8809716072507</v>
       </c>
       <c r="B242" t="s">
+        <v>532</v>
+      </c>
+      <c r="C242" t="s">
         <v>533</v>
       </c>
-      <c r="C242" t="s">
-        <v>534</v>
-      </c>
       <c r="D242" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E242">
         <v>10</v>
@@ -6453,16 +6450,16 @@
         <v>8809716072538</v>
       </c>
       <c r="B243" t="s">
+        <v>534</v>
+      </c>
+      <c r="C243" t="s">
         <v>535</v>
-      </c>
-      <c r="C243" t="s">
-        <v>536</v>
       </c>
       <c r="D243" t="s">
         <v>95</v>
       </c>
       <c r="E243">
-        <v>9</v>
+        <v>25</v>
       </c>
     </row>
     <row r="244" spans="1:5">
@@ -6470,10 +6467,10 @@
         <v>8809716072613</v>
       </c>
       <c r="B244" t="s">
+        <v>536</v>
+      </c>
+      <c r="C244" t="s">
         <v>537</v>
-      </c>
-      <c r="C244" t="s">
-        <v>538</v>
       </c>
       <c r="D244" t="s">
         <v>11</v>
@@ -6487,10 +6484,10 @@
         <v>8809716072637</v>
       </c>
       <c r="B245" t="s">
+        <v>538</v>
+      </c>
+      <c r="C245" t="s">
         <v>539</v>
-      </c>
-      <c r="C245" t="s">
-        <v>540</v>
       </c>
       <c r="D245" t="s">
         <v>32</v>
@@ -6504,10 +6501,10 @@
         <v>8809716072651</v>
       </c>
       <c r="B246" t="s">
+        <v>540</v>
+      </c>
+      <c r="C246" t="s">
         <v>541</v>
-      </c>
-      <c r="C246" t="s">
-        <v>542</v>
       </c>
       <c r="D246" t="s">
         <v>87</v>
@@ -6521,13 +6518,13 @@
         <v>8809716072743</v>
       </c>
       <c r="B247" t="s">
+        <v>542</v>
+      </c>
+      <c r="C247" t="s">
         <v>543</v>
       </c>
-      <c r="C247" t="s">
-        <v>544</v>
-      </c>
       <c r="D247" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E247">
         <v>37</v>
@@ -6538,16 +6535,16 @@
         <v>8809716072835</v>
       </c>
       <c r="B248" t="s">
+        <v>544</v>
+      </c>
+      <c r="C248" t="s">
         <v>545</v>
-      </c>
-      <c r="C248" t="s">
-        <v>546</v>
       </c>
       <c r="D248" t="s">
         <v>90</v>
       </c>
       <c r="E248">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="249" spans="1:5">
@@ -6555,10 +6552,10 @@
         <v>8809716072958</v>
       </c>
       <c r="B249" t="s">
+        <v>546</v>
+      </c>
+      <c r="C249" t="s">
         <v>547</v>
-      </c>
-      <c r="C249" t="s">
-        <v>548</v>
       </c>
       <c r="D249" t="s">
         <v>11</v>
@@ -6572,13 +6569,13 @@
         <v>8809716072989</v>
       </c>
       <c r="B250" t="s">
+        <v>548</v>
+      </c>
+      <c r="C250" t="s">
         <v>549</v>
       </c>
-      <c r="C250" t="s">
-        <v>550</v>
-      </c>
       <c r="D250" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E250">
         <v>40</v>
@@ -6589,16 +6586,16 @@
         <v>8809716073016</v>
       </c>
       <c r="B251" t="s">
+        <v>550</v>
+      </c>
+      <c r="C251" t="s">
         <v>551</v>
       </c>
-      <c r="C251" t="s">
-        <v>552</v>
-      </c>
       <c r="D251" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="E251">
-        <v>5</v>
+        <v>40</v>
       </c>
     </row>
     <row r="252" spans="1:5">
@@ -6606,16 +6603,16 @@
         <v>8809716073047</v>
       </c>
       <c r="B252" t="s">
+        <v>552</v>
+      </c>
+      <c r="C252" t="s">
         <v>553</v>
       </c>
-      <c r="C252" t="s">
-        <v>554</v>
-      </c>
       <c r="D252" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="E252">
-        <v>3</v>
+        <v>30</v>
       </c>
     </row>
     <row r="253" spans="1:5">
@@ -6623,16 +6620,16 @@
         <v>8809716073078</v>
       </c>
       <c r="B253" t="s">
+        <v>554</v>
+      </c>
+      <c r="C253" t="s">
         <v>555</v>
-      </c>
-      <c r="C253" t="s">
-        <v>556</v>
       </c>
       <c r="D253" t="s">
         <v>87</v>
       </c>
       <c r="E253">
-        <v>24</v>
+        <v>25</v>
       </c>
     </row>
     <row r="254" spans="1:5">
@@ -6640,10 +6637,10 @@
         <v>8809716073542</v>
       </c>
       <c r="B254" t="s">
+        <v>556</v>
+      </c>
+      <c r="C254" t="s">
         <v>557</v>
-      </c>
-      <c r="C254" t="s">
-        <v>558</v>
       </c>
       <c r="D254" t="s">
         <v>42</v>
@@ -6657,10 +6654,10 @@
         <v>8809716075003</v>
       </c>
       <c r="B255" t="s">
+        <v>558</v>
+      </c>
+      <c r="C255" t="s">
         <v>559</v>
-      </c>
-      <c r="C255" t="s">
-        <v>560</v>
       </c>
       <c r="D255" t="s">
         <v>87</v>
@@ -6674,13 +6671,13 @@
         <v>8809716075034</v>
       </c>
       <c r="B256" t="s">
+        <v>560</v>
+      </c>
+      <c r="C256" t="s">
         <v>561</v>
       </c>
-      <c r="C256" t="s">
-        <v>562</v>
-      </c>
       <c r="D256" t="s">
-        <v>465</v>
+        <v>464</v>
       </c>
       <c r="E256">
         <v>10</v>
@@ -6691,13 +6688,13 @@
         <v>8809716075065</v>
       </c>
       <c r="B257" t="s">
+        <v>562</v>
+      </c>
+      <c r="C257" t="s">
         <v>563</v>
       </c>
-      <c r="C257" t="s">
+      <c r="D257" t="s">
         <v>564</v>
-      </c>
-      <c r="D257" t="s">
-        <v>565</v>
       </c>
       <c r="E257">
         <v>30</v>
@@ -6708,16 +6705,16 @@
         <v>8809716075096</v>
       </c>
       <c r="B258" t="s">
+        <v>565</v>
+      </c>
+      <c r="C258" t="s">
         <v>566</v>
       </c>
-      <c r="C258" t="s">
-        <v>567</v>
-      </c>
       <c r="D258" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E258">
-        <v>1</v>
+        <v>30</v>
       </c>
     </row>
     <row r="259" spans="1:5">
@@ -6725,13 +6722,13 @@
         <v>8809716075577</v>
       </c>
       <c r="B259" t="s">
+        <v>567</v>
+      </c>
+      <c r="C259" t="s">
         <v>568</v>
       </c>
-      <c r="C259" t="s">
-        <v>569</v>
-      </c>
       <c r="D259" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E259">
         <v>30</v>
@@ -6742,10 +6739,10 @@
         <v>8809716075591</v>
       </c>
       <c r="B260" t="s">
+        <v>569</v>
+      </c>
+      <c r="C260" t="s">
         <v>570</v>
-      </c>
-      <c r="C260" t="s">
-        <v>571</v>
       </c>
       <c r="D260" t="s">
         <v>82</v>
@@ -6759,16 +6756,16 @@
         <v>8809716075669</v>
       </c>
       <c r="B261" t="s">
+        <v>571</v>
+      </c>
+      <c r="C261" t="s">
         <v>572</v>
-      </c>
-      <c r="C261" t="s">
-        <v>573</v>
       </c>
       <c r="D261" t="s">
         <v>48</v>
       </c>
       <c r="E261">
-        <v>2</v>
+        <v>30</v>
       </c>
     </row>
     <row r="262" spans="1:5">
@@ -6776,16 +6773,16 @@
         <v>8809716075690</v>
       </c>
       <c r="B262" t="s">
+        <v>573</v>
+      </c>
+      <c r="C262" t="s">
         <v>574</v>
-      </c>
-      <c r="C262" t="s">
-        <v>575</v>
       </c>
       <c r="D262" t="s">
         <v>68</v>
       </c>
       <c r="E262">
-        <v>5</v>
+        <v>20</v>
       </c>
     </row>
     <row r="263" spans="1:5">
@@ -6793,16 +6790,16 @@
         <v>8809716075720</v>
       </c>
       <c r="B263" t="s">
+        <v>575</v>
+      </c>
+      <c r="C263" t="s">
         <v>576</v>
-      </c>
-      <c r="C263" t="s">
-        <v>577</v>
       </c>
       <c r="D263" t="s">
         <v>8</v>
       </c>
       <c r="E263">
-        <v>4</v>
+        <v>15</v>
       </c>
     </row>
     <row r="264" spans="1:5">
@@ -6810,10 +6807,10 @@
         <v>8809716075751</v>
       </c>
       <c r="B264" t="s">
+        <v>577</v>
+      </c>
+      <c r="C264" t="s">
         <v>578</v>
-      </c>
-      <c r="C264" t="s">
-        <v>579</v>
       </c>
       <c r="D264" t="s">
         <v>35</v>
@@ -6827,10 +6824,10 @@
         <v>887276344379</v>
       </c>
       <c r="B265" t="s">
+        <v>579</v>
+      </c>
+      <c r="C265" t="s">
         <v>580</v>
-      </c>
-      <c r="C265" t="s">
-        <v>581</v>
       </c>
       <c r="D265" t="s">
         <v>53</v>
@@ -6844,10 +6841,10 @@
         <v>887276360331</v>
       </c>
       <c r="B266" t="s">
+        <v>581</v>
+      </c>
+      <c r="C266" t="s">
         <v>582</v>
-      </c>
-      <c r="C266" t="s">
-        <v>583</v>
       </c>
       <c r="D266" t="s">
         <v>40</v>
@@ -6861,10 +6858,10 @@
         <v>887276360409</v>
       </c>
       <c r="B267" t="s">
+        <v>583</v>
+      </c>
+      <c r="C267" t="s">
         <v>584</v>
-      </c>
-      <c r="C267" t="s">
-        <v>585</v>
       </c>
       <c r="D267" t="s">
         <v>90</v>
@@ -6878,10 +6875,10 @@
         <v>887276361574</v>
       </c>
       <c r="B268" t="s">
+        <v>585</v>
+      </c>
+      <c r="C268" t="s">
         <v>586</v>
-      </c>
-      <c r="C268" t="s">
-        <v>587</v>
       </c>
       <c r="D268" t="s">
         <v>40</v>
@@ -6895,10 +6892,10 @@
         <v>887276363875</v>
       </c>
       <c r="B269" t="s">
+        <v>587</v>
+      </c>
+      <c r="C269" t="s">
         <v>588</v>
-      </c>
-      <c r="C269" t="s">
-        <v>589</v>
       </c>
       <c r="D269" t="s">
         <v>42</v>
@@ -6912,13 +6909,13 @@
         <v>887276363882</v>
       </c>
       <c r="B270" t="s">
+        <v>589</v>
+      </c>
+      <c r="C270" t="s">
         <v>590</v>
       </c>
-      <c r="C270" t="s">
-        <v>591</v>
-      </c>
       <c r="D270" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E270">
         <v>10</v>
@@ -6929,16 +6926,16 @@
         <v>887276373492</v>
       </c>
       <c r="B271" t="s">
+        <v>591</v>
+      </c>
+      <c r="C271" t="s">
         <v>592</v>
       </c>
-      <c r="C271" t="s">
-        <v>593</v>
-      </c>
       <c r="D271" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="E271">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="272" spans="1:5">
@@ -6946,13 +6943,13 @@
         <v>887276391830</v>
       </c>
       <c r="B272" t="s">
+        <v>593</v>
+      </c>
+      <c r="C272" t="s">
         <v>594</v>
       </c>
-      <c r="C272" t="s">
-        <v>595</v>
-      </c>
       <c r="D272" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E272">
         <v>17</v>
@@ -6963,13 +6960,13 @@
         <v>887276391861</v>
       </c>
       <c r="B273" t="s">
+        <v>595</v>
+      </c>
+      <c r="C273" t="s">
         <v>596</v>
       </c>
-      <c r="C273" t="s">
-        <v>597</v>
-      </c>
       <c r="D273" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E273">
         <v>11</v>
@@ -6980,16 +6977,16 @@
         <v>887276391915</v>
       </c>
       <c r="B274" t="s">
+        <v>597</v>
+      </c>
+      <c r="C274" t="s">
         <v>598</v>
       </c>
-      <c r="C274" t="s">
-        <v>599</v>
-      </c>
       <c r="D274" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E274">
-        <v>5</v>
+        <v>25</v>
       </c>
     </row>
     <row r="275" spans="1:5">
@@ -6997,13 +6994,13 @@
         <v>887276392479</v>
       </c>
       <c r="B275" t="s">
+        <v>599</v>
+      </c>
+      <c r="C275" t="s">
         <v>600</v>
       </c>
-      <c r="C275" t="s">
-        <v>601</v>
-      </c>
       <c r="D275" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E275">
         <v>38</v>
@@ -7014,13 +7011,13 @@
         <v>887276392516</v>
       </c>
       <c r="B276" t="s">
+        <v>601</v>
+      </c>
+      <c r="C276" t="s">
         <v>602</v>
       </c>
-      <c r="C276" t="s">
+      <c r="D276" t="s">
         <v>603</v>
-      </c>
-      <c r="D276" t="s">
-        <v>604</v>
       </c>
       <c r="E276">
         <v>21</v>
@@ -7031,13 +7028,13 @@
         <v>887276392561</v>
       </c>
       <c r="B277" t="s">
+        <v>604</v>
+      </c>
+      <c r="C277" t="s">
         <v>605</v>
       </c>
-      <c r="C277" t="s">
-        <v>606</v>
-      </c>
       <c r="D277" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="E277">
         <v>20</v>
@@ -7048,16 +7045,16 @@
         <v>887276435336</v>
       </c>
       <c r="B278" t="s">
+        <v>606</v>
+      </c>
+      <c r="C278" t="s">
         <v>607</v>
       </c>
-      <c r="C278" t="s">
-        <v>608</v>
-      </c>
       <c r="D278" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="E278">
-        <v>2</v>
+        <v>25</v>
       </c>
     </row>
     <row r="279" spans="1:5">
@@ -7065,30 +7062,30 @@
         <v>887276435558</v>
       </c>
       <c r="B279" t="s">
+        <v>608</v>
+      </c>
+      <c r="C279" t="s">
         <v>609</v>
       </c>
-      <c r="C279" t="s">
+      <c r="D279" t="s">
         <v>610</v>
       </c>
-      <c r="D279" t="s">
-        <v>611</v>
-      </c>
       <c r="E279">
-        <v>49</v>
+        <v>50</v>
       </c>
     </row>
     <row r="280" spans="1:5">
       <c r="A280" s="4" t="s">
+        <v>611</v>
+      </c>
+      <c r="B280" t="s">
+        <v>611</v>
+      </c>
+      <c r="C280" t="s">
         <v>612</v>
       </c>
-      <c r="B280" t="s">
-        <v>612</v>
-      </c>
-      <c r="C280" t="s">
-        <v>613</v>
-      </c>
       <c r="D280" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="E280">
         <v>25</v>
@@ -7096,33 +7093,33 @@
     </row>
     <row r="281" spans="1:5">
       <c r="A281" s="4" t="s">
+        <v>613</v>
+      </c>
+      <c r="B281" t="s">
+        <v>613</v>
+      </c>
+      <c r="C281" t="s">
         <v>614</v>
-      </c>
-      <c r="B281" t="s">
-        <v>614</v>
-      </c>
-      <c r="C281" t="s">
-        <v>615</v>
       </c>
       <c r="D281" t="s">
         <v>8</v>
       </c>
       <c r="E281">
-        <v>8</v>
+        <v>10</v>
       </c>
     </row>
     <row r="282" spans="1:5">
       <c r="A282" s="4" t="s">
+        <v>615</v>
+      </c>
+      <c r="B282" t="s">
+        <v>615</v>
+      </c>
+      <c r="C282" t="s">
         <v>616</v>
       </c>
-      <c r="B282" t="s">
-        <v>616</v>
-      </c>
-      <c r="C282" t="s">
-        <v>617</v>
-      </c>
       <c r="D282" t="s">
-        <v>98</v>
+        <v>16</v>
       </c>
       <c r="E282">
         <v>16</v>
@@ -7130,33 +7127,33 @@
     </row>
     <row r="283" spans="1:5">
       <c r="A283" s="4" t="s">
+        <v>617</v>
+      </c>
+      <c r="B283" t="s">
+        <v>617</v>
+      </c>
+      <c r="C283" t="s">
         <v>618</v>
-      </c>
-      <c r="B283" t="s">
-        <v>618</v>
-      </c>
-      <c r="C283" t="s">
-        <v>619</v>
       </c>
       <c r="D283" t="s">
         <v>8</v>
       </c>
       <c r="E283">
-        <v>4</v>
+        <v>20</v>
       </c>
     </row>
     <row r="284" spans="1:5">
       <c r="A284" s="4" t="s">
+        <v>619</v>
+      </c>
+      <c r="B284" t="s">
+        <v>619</v>
+      </c>
+      <c r="C284" t="s">
         <v>620</v>
       </c>
-      <c r="B284" t="s">
-        <v>620</v>
-      </c>
-      <c r="C284" t="s">
-        <v>621</v>
-      </c>
       <c r="D284" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="E284">
         <v>40</v>
@@ -7164,64 +7161,64 @@
     </row>
     <row r="285" spans="1:5">
       <c r="A285" s="4" t="s">
+        <v>621</v>
+      </c>
+      <c r="B285" t="s">
+        <v>621</v>
+      </c>
+      <c r="C285" t="s">
         <v>622</v>
       </c>
-      <c r="B285" t="s">
-        <v>622</v>
-      </c>
-      <c r="C285" t="s">
-        <v>623</v>
-      </c>
       <c r="D285" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="E285">
-        <v>2</v>
+        <v>15</v>
       </c>
     </row>
     <row r="286" spans="1:5">
       <c r="A286" s="4" t="s">
+        <v>623</v>
+      </c>
+      <c r="B286" t="s">
+        <v>623</v>
+      </c>
+      <c r="C286" t="s">
         <v>624</v>
       </c>
-      <c r="B286" t="s">
-        <v>624</v>
-      </c>
-      <c r="C286" t="s">
-        <v>625</v>
-      </c>
       <c r="D286" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E286">
-        <v>8</v>
+        <v>35</v>
       </c>
     </row>
     <row r="287" spans="1:5">
       <c r="A287" s="4" t="s">
+        <v>625</v>
+      </c>
+      <c r="B287" t="s">
+        <v>625</v>
+      </c>
+      <c r="C287" t="s">
         <v>626</v>
       </c>
-      <c r="B287" t="s">
-        <v>626</v>
-      </c>
-      <c r="C287" t="s">
-        <v>627</v>
-      </c>
       <c r="D287" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="E287">
-        <v>28</v>
+        <v>30</v>
       </c>
     </row>
     <row r="288" spans="1:5">
       <c r="A288" s="4" t="s">
+        <v>627</v>
+      </c>
+      <c r="B288" t="s">
+        <v>627</v>
+      </c>
+      <c r="C288" t="s">
         <v>628</v>
-      </c>
-      <c r="B288" t="s">
-        <v>628</v>
-      </c>
-      <c r="C288" t="s">
-        <v>629</v>
       </c>
       <c r="D288" t="s">
         <v>42</v>
@@ -7232,13 +7229,13 @@
     </row>
     <row r="289" spans="1:5">
       <c r="A289" s="4" t="s">
+        <v>629</v>
+      </c>
+      <c r="B289" t="s">
+        <v>629</v>
+      </c>
+      <c r="C289" t="s">
         <v>630</v>
-      </c>
-      <c r="B289" t="s">
-        <v>630</v>
-      </c>
-      <c r="C289" t="s">
-        <v>631</v>
       </c>
       <c r="D289" t="s">
         <v>29</v>
@@ -7249,16 +7246,16 @@
     </row>
     <row r="290" spans="1:5">
       <c r="A290" s="4" t="s">
+        <v>631</v>
+      </c>
+      <c r="B290" t="s">
+        <v>631</v>
+      </c>
+      <c r="C290" t="s">
         <v>632</v>
       </c>
-      <c r="B290" t="s">
-        <v>632</v>
-      </c>
-      <c r="C290" t="s">
-        <v>633</v>
-      </c>
       <c r="D290" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="E290">
         <v>50</v>

</xml_diff>